<commit_message>
Update data: 8 May 2020
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="16">
   <si>
     <t>date</t>
   </si>
@@ -395,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -466,6 +466,20 @@
         <v>1547</v>
       </c>
     </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>109.4</v>
+      </c>
+      <c r="D5">
+        <v>2418.3000000000002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -473,10 +487,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -500,142 +514,142 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1">
-        <v>43891</v>
+        <v>43831</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C2">
-        <v>-4.3</v>
+        <v>0.3</v>
       </c>
       <c r="D2">
-        <v>28.9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1">
-        <v>43891</v>
+        <v>43831</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3">
-        <v>-1.3</v>
+        <v>-18.8</v>
       </c>
       <c r="D3">
-        <v>7.4</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
-        <v>43891</v>
+        <v>43831</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4">
-        <v>42.7</v>
+        <v>10.7</v>
       </c>
       <c r="D4">
-        <v>44.1</v>
+        <v>37.200000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1">
-        <v>43891</v>
+        <v>43831</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5">
-        <v>8.8000000000000007</v>
+        <v>-7</v>
       </c>
       <c r="D5">
-        <v>33.299999999999997</v>
+        <v>29.2</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1">
-        <v>43891</v>
+        <v>43831</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6">
-        <v>54.7</v>
+        <v>-4.2</v>
       </c>
       <c r="D6">
-        <v>362.8</v>
+        <v>232.7</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1">
-        <v>43891</v>
+        <v>43831</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7">
-        <v>27.5</v>
+        <v>-7.4</v>
       </c>
       <c r="D7">
-        <v>585.6</v>
+        <v>415.3</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1">
-        <v>43891</v>
+        <v>43831</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8">
-        <v>26.9</v>
+        <v>-7.5</v>
       </c>
       <c r="D8">
-        <v>43.9</v>
+        <v>35.700000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1">
-        <v>43891</v>
+        <v>43831</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9">
-        <v>43.1</v>
+        <v>9.4</v>
       </c>
       <c r="D9">
-        <v>43.8</v>
+        <v>37.299999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1">
-        <v>43891</v>
+        <v>43831</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10">
-        <v>22.7</v>
+        <v>7</v>
       </c>
       <c r="D10">
-        <v>210.5</v>
+        <v>181.7</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1">
-        <v>43891</v>
+        <v>43831</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
       <c r="C11">
-        <v>48.3</v>
+        <v>-5.2</v>
       </c>
       <c r="D11">
-        <v>186.7</v>
+        <v>118.8</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -780,142 +794,282 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1">
-        <v>43831</v>
+        <v>43891</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C22">
-        <v>0.3</v>
+        <v>-4.3</v>
       </c>
       <c r="D22">
-        <v>30</v>
+        <v>28.9</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1">
-        <v>43831</v>
+        <v>43891</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
       <c r="C23">
-        <v>-18.8</v>
+        <v>-1.3</v>
       </c>
       <c r="D23">
-        <v>6.5</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1">
-        <v>43831</v>
+        <v>43891</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
       </c>
       <c r="C24">
-        <v>10.7</v>
+        <v>42.7</v>
       </c>
       <c r="D24">
-        <v>37.200000000000003</v>
+        <v>44.1</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1">
-        <v>43831</v>
+        <v>43891</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
       </c>
       <c r="C25">
-        <v>-7</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="D25">
-        <v>29.2</v>
+        <v>33.299999999999997</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1">
-        <v>43831</v>
+        <v>43891</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
       </c>
       <c r="C26">
-        <v>-4.2</v>
+        <v>54.7</v>
       </c>
       <c r="D26">
-        <v>232.7</v>
+        <v>362.8</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1">
-        <v>43831</v>
+        <v>43891</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
       <c r="C27">
-        <v>-7.4</v>
+        <v>27.5</v>
       </c>
       <c r="D27">
-        <v>415.3</v>
+        <v>585.6</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1">
-        <v>43831</v>
+        <v>43891</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
       </c>
       <c r="C28">
-        <v>-7.5</v>
+        <v>26.9</v>
       </c>
       <c r="D28">
-        <v>35.700000000000003</v>
+        <v>43.9</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1">
-        <v>43831</v>
+        <v>43891</v>
       </c>
       <c r="B29" t="s">
         <v>11</v>
       </c>
       <c r="C29">
-        <v>9.4</v>
+        <v>43.1</v>
       </c>
       <c r="D29">
-        <v>37.299999999999997</v>
+        <v>43.8</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1">
-        <v>43831</v>
+        <v>43891</v>
       </c>
       <c r="B30" t="s">
         <v>12</v>
       </c>
       <c r="C30">
-        <v>7</v>
+        <v>22.7</v>
       </c>
       <c r="D30">
-        <v>181.7</v>
+        <v>210.5</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1">
-        <v>43831</v>
+        <v>43891</v>
       </c>
       <c r="B31" t="s">
         <v>13</v>
       </c>
       <c r="C31">
-        <v>-5.2</v>
+        <v>48.3</v>
       </c>
       <c r="D31">
-        <v>118.8</v>
+        <v>186.7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32">
+        <v>17</v>
+      </c>
+      <c r="D32">
+        <v>35.799999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1">
+        <v>43923</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33">
+        <v>15.1</v>
+      </c>
+      <c r="D33">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1">
+        <v>43924</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34">
+        <v>55.6</v>
+      </c>
+      <c r="D34">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1">
+        <v>43925</v>
+      </c>
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35">
+        <v>52.8</v>
+      </c>
+      <c r="D35">
+        <v>47.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1">
+        <v>43926</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36">
+        <v>224.2</v>
+      </c>
+      <c r="D36">
+        <v>729.4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37">
+        <v>76.900000000000006</v>
+      </c>
+      <c r="D37">
+        <v>822.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38">
+        <v>107.6</v>
+      </c>
+      <c r="D38">
+        <v>73.7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1">
+        <v>43929</v>
+      </c>
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39">
+        <v>92.6</v>
+      </c>
+      <c r="D39">
+        <v>64.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="D40">
+        <v>304.3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1">
+        <v>43931</v>
+      </c>
+      <c r="B41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41">
+        <v>125.1</v>
+      </c>
+      <c r="D41">
+        <v>278.39999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data: 5 June 2020
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="16">
   <si>
     <t>date</t>
   </si>
@@ -98,9 +98,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,15 +397,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
   </cols>
@@ -480,17 +482,32 @@
         <v>2418.3000000000002</v>
       </c>
     </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>139.80000000000001</v>
+      </c>
+      <c r="D6">
+        <v>2619.1999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -653,16 +670,16 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="1">
+      <c r="A12" s="2">
         <v>43862</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>-1.9</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <v>30.3</v>
       </c>
     </row>
@@ -793,16 +810,16 @@
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="1">
+      <c r="A22" s="2">
         <v>43891</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="3">
         <v>-4.3</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="3">
         <v>28.9</v>
       </c>
     </row>
@@ -948,7 +965,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1">
-        <v>43923</v>
+        <v>43922</v>
       </c>
       <c r="B33" t="s">
         <v>5</v>
@@ -962,7 +979,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1">
-        <v>43924</v>
+        <v>43922</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
@@ -976,7 +993,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1">
-        <v>43925</v>
+        <v>43922</v>
       </c>
       <c r="B35" t="s">
         <v>7</v>
@@ -990,7 +1007,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1">
-        <v>43926</v>
+        <v>43922</v>
       </c>
       <c r="B36" t="s">
         <v>8</v>
@@ -1004,7 +1021,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1">
-        <v>43927</v>
+        <v>43922</v>
       </c>
       <c r="B37" t="s">
         <v>9</v>
@@ -1018,7 +1035,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1">
-        <v>43928</v>
+        <v>43922</v>
       </c>
       <c r="B38" t="s">
         <v>10</v>
@@ -1032,7 +1049,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1">
-        <v>43929</v>
+        <v>43922</v>
       </c>
       <c r="B39" t="s">
         <v>11</v>
@@ -1046,7 +1063,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1">
-        <v>43930</v>
+        <v>43922</v>
       </c>
       <c r="B40" t="s">
         <v>12</v>
@@ -1060,7 +1077,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1">
-        <v>43931</v>
+        <v>43922</v>
       </c>
       <c r="B41" t="s">
         <v>13</v>
@@ -1070,6 +1087,146 @@
       </c>
       <c r="D41">
         <v>278.39999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42">
+        <v>20.2</v>
+      </c>
+      <c r="D42">
+        <v>38.700000000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <v>52.6</v>
+      </c>
+      <c r="D43">
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44">
+        <v>89.3</v>
+      </c>
+      <c r="D44">
+        <v>63.4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45">
+        <v>68.5</v>
+      </c>
+      <c r="D45">
+        <v>48.2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46">
+        <v>166.5</v>
+      </c>
+      <c r="D46">
+        <v>603.9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47">
+        <v>145.19999999999999</v>
+      </c>
+      <c r="D47">
+        <v>1003.4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48">
+        <v>112</v>
+      </c>
+      <c r="D48">
+        <v>74.400000000000006</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49">
+        <v>125.5</v>
+      </c>
+      <c r="D49">
+        <v>72.400000000000006</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B50" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50">
+        <v>116</v>
+      </c>
+      <c r="D50">
+        <v>365.1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B51" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51">
+        <v>185.3</v>
+      </c>
+      <c r="D51">
+        <v>338.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data: 11 July 2020
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="16">
   <si>
     <t>date</t>
   </si>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -496,6 +496,20 @@
         <v>2619.1999999999998</v>
       </c>
     </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>118.4</v>
+      </c>
+      <c r="D7">
+        <v>1122.9000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -504,10 +518,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1229,6 +1243,146 @@
         <v>338.1</v>
       </c>
     </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="D52">
+        <v>33.9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53">
+        <v>69.2</v>
+      </c>
+      <c r="D53">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B54" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54">
+        <v>91.1</v>
+      </c>
+      <c r="D54">
+        <v>33.799999999999997</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B55" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55">
+        <v>25.6</v>
+      </c>
+      <c r="D55">
+        <v>30.8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56">
+        <v>116.4</v>
+      </c>
+      <c r="D56">
+        <v>224.3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B57" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57">
+        <v>119</v>
+      </c>
+      <c r="D57">
+        <v>430.8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B58" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58">
+        <v>77.2</v>
+      </c>
+      <c r="D58">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B59" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59">
+        <v>121.8</v>
+      </c>
+      <c r="D59">
+        <v>31.7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B60" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60">
+        <v>127.9</v>
+      </c>
+      <c r="D60">
+        <v>167.8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B61" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61">
+        <v>180.9</v>
+      </c>
+      <c r="D61">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update data: 7 August 2020
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="16">
   <si>
     <t>date</t>
   </si>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -507,7 +507,21 @@
         <v>118.4</v>
       </c>
       <c r="D7">
-        <v>1122.9000000000001</v>
+        <v>2452.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>44013</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>89.3</v>
+      </c>
+      <c r="D8">
+        <v>2183.6</v>
       </c>
     </row>
   </sheetData>
@@ -518,10 +532,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1254,7 +1268,7 @@
         <v>18.600000000000001</v>
       </c>
       <c r="D52">
-        <v>33.9</v>
+        <v>40.200000000000003</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1268,7 +1282,7 @@
         <v>69.2</v>
       </c>
       <c r="D53">
-        <v>7.8</v>
+        <v>13.2</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1282,7 +1296,7 @@
         <v>91.1</v>
       </c>
       <c r="D54">
-        <v>33.799999999999997</v>
+        <v>64.599999999999994</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1296,7 +1310,7 @@
         <v>25.6</v>
       </c>
       <c r="D55">
-        <v>30.8</v>
+        <v>38.700000000000003</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1310,7 +1324,7 @@
         <v>116.4</v>
       </c>
       <c r="D56">
-        <v>224.3</v>
+        <v>485.3</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1324,7 +1338,7 @@
         <v>119</v>
       </c>
       <c r="D57">
-        <v>430.8</v>
+        <v>943.3</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1338,7 +1352,7 @@
         <v>77.2</v>
       </c>
       <c r="D58">
-        <v>39</v>
+        <v>69.099999999999994</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1352,7 +1366,7 @@
         <v>121.8</v>
       </c>
       <c r="D59">
-        <v>31.7</v>
+        <v>70.3</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1366,7 +1380,7 @@
         <v>127.9</v>
       </c>
       <c r="D60">
-        <v>167.8</v>
+        <v>382.5</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1380,7 +1394,147 @@
         <v>180.9</v>
       </c>
       <c r="D61">
-        <v>123</v>
+        <v>345.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="1">
+        <v>44013</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="D62">
+        <v>38.6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="1">
+        <v>44013</v>
+      </c>
+      <c r="B63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63">
+        <v>37.5</v>
+      </c>
+      <c r="D63">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="1">
+        <v>44013</v>
+      </c>
+      <c r="B64" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64">
+        <v>41.6</v>
+      </c>
+      <c r="D64">
+        <v>52.8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="1">
+        <v>44013</v>
+      </c>
+      <c r="B65" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65">
+        <v>15.2</v>
+      </c>
+      <c r="D65">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="1">
+        <v>44013</v>
+      </c>
+      <c r="B66" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66">
+        <v>94.7</v>
+      </c>
+      <c r="D66">
+        <v>436.8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="1">
+        <v>44013</v>
+      </c>
+      <c r="B67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67">
+        <v>98.2</v>
+      </c>
+      <c r="D67">
+        <v>886.6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="1">
+        <v>44013</v>
+      </c>
+      <c r="B68" t="s">
+        <v>10</v>
+      </c>
+      <c r="C68">
+        <v>41.5</v>
+      </c>
+      <c r="D68">
+        <v>56.3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="1">
+        <v>44013</v>
+      </c>
+      <c r="B69" t="s">
+        <v>11</v>
+      </c>
+      <c r="C69">
+        <v>59.9</v>
+      </c>
+      <c r="D69">
+        <v>53.1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="1">
+        <v>44013</v>
+      </c>
+      <c r="B70" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70">
+        <v>77.2</v>
+      </c>
+      <c r="D70">
+        <v>316.10000000000002</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="1">
+        <v>44013</v>
+      </c>
+      <c r="B71" t="s">
+        <v>13</v>
+      </c>
+      <c r="C71">
+        <v>145.9</v>
+      </c>
+      <c r="D71">
+        <v>295.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data: 4 September 2020
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="16">
   <si>
     <t>date</t>
   </si>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -524,6 +524,20 @@
         <v>2183.6</v>
       </c>
     </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>44044</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>76.5</v>
+      </c>
+      <c r="D9">
+        <v>2046.9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -532,10 +546,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1537,6 +1551,146 @@
         <v>295.3</v>
       </c>
     </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="1">
+        <v>44044</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72">
+        <v>-3.6</v>
+      </c>
+      <c r="D72">
+        <v>32.1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="1">
+        <v>44044</v>
+      </c>
+      <c r="B73" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73">
+        <v>19.7</v>
+      </c>
+      <c r="D73">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="1">
+        <v>44044</v>
+      </c>
+      <c r="B74" t="s">
+        <v>6</v>
+      </c>
+      <c r="C74">
+        <v>27.3</v>
+      </c>
+      <c r="D74">
+        <v>50.8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="1">
+        <v>44044</v>
+      </c>
+      <c r="B75" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75">
+        <v>9</v>
+      </c>
+      <c r="D75">
+        <v>36.200000000000003</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="1">
+        <v>44044</v>
+      </c>
+      <c r="B76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76">
+        <v>83.6</v>
+      </c>
+      <c r="D76">
+        <v>398.4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="1">
+        <v>44044</v>
+      </c>
+      <c r="B77" t="s">
+        <v>9</v>
+      </c>
+      <c r="C77">
+        <v>90</v>
+      </c>
+      <c r="D77">
+        <v>841.4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="1">
+        <v>44044</v>
+      </c>
+      <c r="B78" t="s">
+        <v>10</v>
+      </c>
+      <c r="C78">
+        <v>45.8</v>
+      </c>
+      <c r="D78">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="1">
+        <v>44044</v>
+      </c>
+      <c r="B79" t="s">
+        <v>11</v>
+      </c>
+      <c r="C79">
+        <v>53.9</v>
+      </c>
+      <c r="D79">
+        <v>47.7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="1">
+        <v>44044</v>
+      </c>
+      <c r="B80" t="s">
+        <v>12</v>
+      </c>
+      <c r="C80">
+        <v>59.2</v>
+      </c>
+      <c r="D80">
+        <v>290.39999999999998</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="1">
+        <v>44044</v>
+      </c>
+      <c r="B81" t="s">
+        <v>13</v>
+      </c>
+      <c r="C81">
+        <v>112.5</v>
+      </c>
+      <c r="D81">
+        <v>284.89999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update data: 9 October 2020
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="16">
   <si>
     <t>date</t>
   </si>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -538,6 +538,20 @@
         <v>2046.9</v>
       </c>
     </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>44075</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>65.3</v>
+      </c>
+      <c r="D10">
+        <v>1832.6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -546,10 +560,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1691,6 +1705,146 @@
         <v>284.89999999999998</v>
       </c>
     </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="1">
+        <v>44075</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C82">
+        <v>30.9</v>
+      </c>
+      <c r="D82">
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="1">
+        <v>44075</v>
+      </c>
+      <c r="B83" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83">
+        <v>14.9</v>
+      </c>
+      <c r="D83">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="1">
+        <v>44075</v>
+      </c>
+      <c r="B84" t="s">
+        <v>6</v>
+      </c>
+      <c r="C84">
+        <v>6.9</v>
+      </c>
+      <c r="D84">
+        <v>38.9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="1">
+        <v>44075</v>
+      </c>
+      <c r="B85" t="s">
+        <v>7</v>
+      </c>
+      <c r="C85">
+        <v>28.9</v>
+      </c>
+      <c r="D85">
+        <v>40.6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="1">
+        <v>44075</v>
+      </c>
+      <c r="B86" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86">
+        <v>52.2</v>
+      </c>
+      <c r="D86">
+        <v>341.9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="1">
+        <v>44075</v>
+      </c>
+      <c r="B87" t="s">
+        <v>9</v>
+      </c>
+      <c r="C87">
+        <v>80.2</v>
+      </c>
+      <c r="D87">
+        <v>757.4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="1">
+        <v>44075</v>
+      </c>
+      <c r="B88" t="s">
+        <v>10</v>
+      </c>
+      <c r="C88">
+        <v>49.8</v>
+      </c>
+      <c r="D88">
+        <v>49.3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="1">
+        <v>44075</v>
+      </c>
+      <c r="B89" t="s">
+        <v>11</v>
+      </c>
+      <c r="C89">
+        <v>26.6</v>
+      </c>
+      <c r="D89">
+        <v>41.4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="1">
+        <v>44075</v>
+      </c>
+      <c r="B90" t="s">
+        <v>12</v>
+      </c>
+      <c r="C90">
+        <v>77.7</v>
+      </c>
+      <c r="D90">
+        <v>293.2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="1">
+        <v>44075</v>
+      </c>
+      <c r="B91" t="s">
+        <v>13</v>
+      </c>
+      <c r="C91">
+        <v>73.7</v>
+      </c>
+      <c r="D91">
+        <v>223.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update data: 6 November 2020
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="16">
   <si>
     <t>date</t>
   </si>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -552,6 +552,20 @@
         <v>1832.6</v>
       </c>
     </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>44105</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>60.9</v>
+      </c>
+      <c r="D11">
+        <v>1816.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -560,10 +574,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1845,6 +1859,146 @@
         <v>223.7</v>
       </c>
     </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="1">
+        <v>44105</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C92">
+        <v>15.5</v>
+      </c>
+      <c r="D92">
+        <v>32.700000000000003</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="1">
+        <v>44105</v>
+      </c>
+      <c r="B93" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93">
+        <v>19.7</v>
+      </c>
+      <c r="D93">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="1">
+        <v>44105</v>
+      </c>
+      <c r="B94" t="s">
+        <v>6</v>
+      </c>
+      <c r="C94">
+        <v>6.6</v>
+      </c>
+      <c r="D94">
+        <v>43.8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="1">
+        <v>44105</v>
+      </c>
+      <c r="B95" t="s">
+        <v>7</v>
+      </c>
+      <c r="C95">
+        <v>27.3</v>
+      </c>
+      <c r="D95">
+        <v>39.6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="1">
+        <v>44105</v>
+      </c>
+      <c r="B96" t="s">
+        <v>8</v>
+      </c>
+      <c r="C96">
+        <v>53.3</v>
+      </c>
+      <c r="D96">
+        <v>354.2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="1">
+        <v>44105</v>
+      </c>
+      <c r="B97" t="s">
+        <v>9</v>
+      </c>
+      <c r="C97">
+        <v>81.3</v>
+      </c>
+      <c r="D97">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="1">
+        <v>44105</v>
+      </c>
+      <c r="B98" t="s">
+        <v>10</v>
+      </c>
+      <c r="C98">
+        <v>36.5</v>
+      </c>
+      <c r="D98">
+        <v>49.7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="1">
+        <v>44105</v>
+      </c>
+      <c r="B99" t="s">
+        <v>11</v>
+      </c>
+      <c r="C99">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="D99">
+        <v>38.200000000000003</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="1">
+        <v>44105</v>
+      </c>
+      <c r="B100" t="s">
+        <v>12</v>
+      </c>
+      <c r="C100">
+        <v>56.7</v>
+      </c>
+      <c r="D100">
+        <v>267.10000000000002</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="1">
+        <v>44105</v>
+      </c>
+      <c r="B101" t="s">
+        <v>13</v>
+      </c>
+      <c r="C101">
+        <v>67.2</v>
+      </c>
+      <c r="D101">
+        <v>215</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update data: 4 December 2020
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="16">
   <si>
     <t>date</t>
   </si>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A12" sqref="A12:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -566,6 +566,20 @@
         <v>1816.8</v>
       </c>
     </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>45.6</v>
+      </c>
+      <c r="D12">
+        <v>1735.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -574,10 +588,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102:D111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1999,6 +2013,146 @@
         <v>215</v>
       </c>
     </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C102">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D102">
+        <v>31.3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B103" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103">
+        <v>27.5</v>
+      </c>
+      <c r="D103">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B104" t="s">
+        <v>6</v>
+      </c>
+      <c r="C104">
+        <v>-19.100000000000001</v>
+      </c>
+      <c r="D104">
+        <v>32.200000000000003</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B105" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105">
+        <v>24.4</v>
+      </c>
+      <c r="D105">
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B106" t="s">
+        <v>8</v>
+      </c>
+      <c r="C106">
+        <v>29.4</v>
+      </c>
+      <c r="D106">
+        <v>329.7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B107" t="s">
+        <v>9</v>
+      </c>
+      <c r="C107">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="D107">
+        <v>733.7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B108" t="s">
+        <v>10</v>
+      </c>
+      <c r="C108">
+        <v>32.6</v>
+      </c>
+      <c r="D108">
+        <v>50.9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B109" t="s">
+        <v>11</v>
+      </c>
+      <c r="C109">
+        <v>16.5</v>
+      </c>
+      <c r="D109">
+        <v>41.7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B110" t="s">
+        <v>12</v>
+      </c>
+      <c r="C110">
+        <v>51.6</v>
+      </c>
+      <c r="D110">
+        <v>276.7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="1">
+        <v>44136</v>
+      </c>
+      <c r="B111" t="s">
+        <v>13</v>
+      </c>
+      <c r="C111">
+        <v>43</v>
+      </c>
+      <c r="D111">
+        <v>192.4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update data: 8 January 2021
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="16">
   <si>
     <t>date</t>
   </si>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:D12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -580,6 +580,20 @@
         <v>1735.2</v>
       </c>
     </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>53.6</v>
+      </c>
+      <c r="D13">
+        <v>1755.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -588,10 +602,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D111"/>
+  <dimension ref="A1:D121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102:D111"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2153,6 +2167,146 @@
         <v>192.4</v>
       </c>
     </row>
+    <row r="112" spans="1:4">
+      <c r="A112" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C112">
+        <v>6.1</v>
+      </c>
+      <c r="D112">
+        <v>31.4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B113" t="s">
+        <v>5</v>
+      </c>
+      <c r="C113">
+        <v>24.6</v>
+      </c>
+      <c r="D113">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B114" t="s">
+        <v>6</v>
+      </c>
+      <c r="C114">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D114">
+        <v>43.4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B115" t="s">
+        <v>7</v>
+      </c>
+      <c r="C115">
+        <v>26.8</v>
+      </c>
+      <c r="D115">
+        <v>36.4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B116" t="s">
+        <v>8</v>
+      </c>
+      <c r="C116">
+        <v>26.9</v>
+      </c>
+      <c r="D116">
+        <v>305.8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B117" t="s">
+        <v>9</v>
+      </c>
+      <c r="C117">
+        <v>80</v>
+      </c>
+      <c r="D117">
+        <v>762.5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B118" t="s">
+        <v>10</v>
+      </c>
+      <c r="C118">
+        <v>61.9</v>
+      </c>
+      <c r="D118">
+        <v>55.7</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B119" t="s">
+        <v>11</v>
+      </c>
+      <c r="C119">
+        <v>33.5</v>
+      </c>
+      <c r="D119">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B120" t="s">
+        <v>12</v>
+      </c>
+      <c r="C120">
+        <v>53.9</v>
+      </c>
+      <c r="D120">
+        <v>271.39999999999998</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B121" t="s">
+        <v>13</v>
+      </c>
+      <c r="C121">
+        <v>51.3</v>
+      </c>
+      <c r="D121">
+        <v>193.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update data: 5 February 2021
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="16">
   <si>
     <t>date</t>
   </si>
@@ -397,15 +397,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
   </cols>
@@ -592,6 +592,20 @@
       </c>
       <c r="D13">
         <v>1755.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>67</v>
+      </c>
+      <c r="D14">
+        <v>1899</v>
       </c>
     </row>
   </sheetData>
@@ -602,10 +616,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="C132" sqref="C132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2307,6 +2321,146 @@
         <v>193.7</v>
       </c>
     </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C122">
+        <v>2.8</v>
+      </c>
+      <c r="D122">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B123" t="s">
+        <v>5</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+      <c r="D123">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B124" t="s">
+        <v>6</v>
+      </c>
+      <c r="C124">
+        <v>10.5</v>
+      </c>
+      <c r="D124">
+        <v>42.1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B125" t="s">
+        <v>7</v>
+      </c>
+      <c r="C125">
+        <v>14.5</v>
+      </c>
+      <c r="D125">
+        <v>34.700000000000003</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B126" t="s">
+        <v>8</v>
+      </c>
+      <c r="C126">
+        <v>70.8</v>
+      </c>
+      <c r="D126">
+        <v>394.6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B127" t="s">
+        <v>9</v>
+      </c>
+      <c r="C127">
+        <v>93.1</v>
+      </c>
+      <c r="D127">
+        <v>802.4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B128" t="s">
+        <v>10</v>
+      </c>
+      <c r="C128">
+        <v>51.4</v>
+      </c>
+      <c r="D128">
+        <v>54.8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B129" t="s">
+        <v>11</v>
+      </c>
+      <c r="C129">
+        <v>13.7</v>
+      </c>
+      <c r="D129">
+        <v>42.3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B130" t="s">
+        <v>12</v>
+      </c>
+      <c r="C130">
+        <v>44.4</v>
+      </c>
+      <c r="D130">
+        <v>262.7</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B131" t="s">
+        <v>13</v>
+      </c>
+      <c r="C131">
+        <v>76.2</v>
+      </c>
+      <c r="D131">
+        <v>226.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update data: 12 March 2021
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="16">
   <si>
     <t>date</t>
   </si>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -608,6 +608,20 @@
         <v>1899</v>
       </c>
     </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>45.3</v>
+      </c>
+      <c r="D15">
+        <v>1665.1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -616,10 +630,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D131"/>
+  <dimension ref="A1:D141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2461,6 +2475,146 @@
         <v>226.2</v>
       </c>
     </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C132">
+        <v>18</v>
+      </c>
+      <c r="D132">
+        <v>37.299999999999997</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B133" t="s">
+        <v>5</v>
+      </c>
+      <c r="C133">
+        <v>11.3</v>
+      </c>
+      <c r="D133">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B134" t="s">
+        <v>6</v>
+      </c>
+      <c r="C134">
+        <v>1</v>
+      </c>
+      <c r="D134">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B135" t="s">
+        <v>7</v>
+      </c>
+      <c r="C135">
+        <v>22.4</v>
+      </c>
+      <c r="D135">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B136" t="s">
+        <v>8</v>
+      </c>
+      <c r="C136">
+        <v>41.8</v>
+      </c>
+      <c r="D136">
+        <v>289.39999999999998</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B137" t="s">
+        <v>9</v>
+      </c>
+      <c r="C137">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="D137">
+        <v>726.5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B138" t="s">
+        <v>10</v>
+      </c>
+      <c r="C138">
+        <v>30.9</v>
+      </c>
+      <c r="D138">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B139" t="s">
+        <v>11</v>
+      </c>
+      <c r="C139">
+        <v>11.9</v>
+      </c>
+      <c r="D139">
+        <v>43.1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B140" t="s">
+        <v>12</v>
+      </c>
+      <c r="C140">
+        <v>32.5</v>
+      </c>
+      <c r="D140">
+        <v>242.1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" s="1">
+        <v>44228</v>
+      </c>
+      <c r="B141" t="s">
+        <v>13</v>
+      </c>
+      <c r="C141">
+        <v>38</v>
+      </c>
+      <c r="D141">
+        <v>195.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update data: 14 April 2021
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>province</t>
+  </si>
+  <si>
+    <t>unemployment_2019</t>
   </si>
 </sst>
 </file>
@@ -397,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -410,7 +413,7 @@
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -423,8 +426,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>43831</v>
       </c>
@@ -432,14 +438,17 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>-3.3</v>
+        <f>(D2-E2)/E2*100</f>
+        <v>-3.7344398340249074</v>
       </c>
       <c r="D2">
-        <f>1124.4</f>
-        <v>1124.4000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>1136.8</v>
+      </c>
+      <c r="E2">
+        <v>1180.9000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>43862</v>
       </c>
@@ -447,14 +456,17 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>-2.2999999999999998</v>
+        <f t="shared" ref="C3:C16" si="0">(D3-E3)/E3*100</f>
+        <v>-2.6758409785932722</v>
       </c>
       <c r="D3">
-        <f>1133.8</f>
-        <v>1133.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>1145.7</v>
+      </c>
+      <c r="E3">
+        <v>1177.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>43891</v>
       </c>
@@ -462,13 +474,17 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>33.9</v>
+        <f t="shared" si="0"/>
+        <v>32.894286691755035</v>
       </c>
       <c r="D4">
-        <v>1547</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>1553.8</v>
+      </c>
+      <c r="E4">
+        <v>1169.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>43922</v>
       </c>
@@ -476,13 +492,17 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>109.4</v>
+        <f t="shared" si="0"/>
+        <v>109.43525580598165</v>
       </c>
       <c r="D5">
-        <v>2418.3000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>2443.9</v>
+      </c>
+      <c r="E5">
+        <v>1166.9000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>43952</v>
       </c>
@@ -490,13 +510,17 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>139.80000000000001</v>
+        <f t="shared" si="0"/>
+        <v>138.64301389904904</v>
       </c>
       <c r="D6">
-        <v>2619.1999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>2609.8000000000002</v>
+      </c>
+      <c r="E6">
+        <v>1093.5999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>43983</v>
       </c>
@@ -504,13 +528,17 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>118.4</v>
+        <f t="shared" si="0"/>
+        <v>119.55634427684119</v>
       </c>
       <c r="D7">
-        <v>2452.6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>2474.4</v>
+      </c>
+      <c r="E7">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>44013</v>
       </c>
@@ -518,13 +546,17 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>89.3</v>
+        <f t="shared" si="0"/>
+        <v>87.316570840127028</v>
       </c>
       <c r="D8">
-        <v>2183.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>2182.8000000000002</v>
+      </c>
+      <c r="E8">
+        <v>1165.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>44044</v>
       </c>
@@ -532,13 +564,17 @@
         <v>2</v>
       </c>
       <c r="C9">
-        <v>76.5</v>
+        <f t="shared" si="0"/>
+        <v>74.638789733129386</v>
       </c>
       <c r="D9">
-        <v>2046.9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>2054.8000000000002</v>
+      </c>
+      <c r="E9">
+        <v>1176.5999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>44075</v>
       </c>
@@ -546,13 +582,17 @@
         <v>2</v>
       </c>
       <c r="C10">
-        <v>65.3</v>
+        <f t="shared" si="0"/>
+        <v>65.26147278548558</v>
       </c>
       <c r="D10">
-        <v>1832.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>1858.2</v>
+      </c>
+      <c r="E10">
+        <v>1124.4000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>44105</v>
       </c>
@@ -560,13 +600,17 @@
         <v>2</v>
       </c>
       <c r="C11">
-        <v>60.9</v>
+        <f t="shared" si="0"/>
+        <v>61.033028812368229</v>
       </c>
       <c r="D11">
-        <v>1816.8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>1833.2</v>
+      </c>
+      <c r="E11">
+        <v>1138.4000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>44136</v>
       </c>
@@ -574,13 +618,17 @@
         <v>2</v>
       </c>
       <c r="C12">
-        <v>45.6</v>
+        <f t="shared" si="0"/>
+        <v>45.779302267213254</v>
       </c>
       <c r="D12">
-        <v>1735.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>1742.5</v>
+      </c>
+      <c r="E12">
+        <v>1195.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>44166</v>
       </c>
@@ -588,13 +636,17 @@
         <v>2</v>
       </c>
       <c r="C13">
-        <v>53.6</v>
+        <f t="shared" si="0"/>
+        <v>54.42674327500653</v>
       </c>
       <c r="D13">
-        <v>1755.8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>1773.9</v>
+      </c>
+      <c r="E13">
+        <v>1148.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>44197</v>
       </c>
@@ -602,13 +654,17 @@
         <v>2</v>
       </c>
       <c r="C14">
-        <v>67</v>
+        <f t="shared" si="0"/>
+        <v>60.809552036582261</v>
       </c>
       <c r="D14">
         <v>1899</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14">
+        <v>1180.9000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>44228</v>
       </c>
@@ -616,10 +672,32 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <v>45.3</v>
+        <f t="shared" si="0"/>
+        <v>41.44580360176689</v>
       </c>
       <c r="D15">
         <v>1665.1</v>
+      </c>
+      <c r="E15">
+        <v>1177.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>29.721176873075606</v>
+      </c>
+      <c r="D16">
+        <v>1516.7</v>
+      </c>
+      <c r="E16">
+        <v>1169.2</v>
       </c>
     </row>
   </sheetData>
@@ -630,10 +708,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D141"/>
+  <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D146" sqref="D146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -641,7 +719,7 @@
     <col min="1" max="1" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -654,8 +732,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>43831</v>
       </c>
@@ -663,13 +744,17 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>0.3</v>
+        <f>(D2-E2)/E2*100</f>
+        <v>0.95846645367412364</v>
       </c>
       <c r="D2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>31.6</v>
+      </c>
+      <c r="E2">
+        <v>31.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -677,13 +762,17 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>-18.8</v>
+        <f>(D3-E3)/E3*100</f>
+        <v>-18.292682926829258</v>
       </c>
       <c r="D3">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>6.7</v>
+      </c>
+      <c r="E3">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>43831</v>
       </c>
@@ -691,13 +780,17 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>10.7</v>
+        <f t="shared" ref="C4:C67" si="0">(D4-E4)/E4*100</f>
+        <v>8.5470085470085468</v>
       </c>
       <c r="D4">
-        <v>37.200000000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>38.1</v>
+      </c>
+      <c r="E4">
+        <v>35.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>43831</v>
       </c>
@@ -705,13 +798,17 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>-7</v>
+        <f t="shared" si="0"/>
+        <v>-6.1919504643962746</v>
       </c>
       <c r="D5">
-        <v>29.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>30.3</v>
+      </c>
+      <c r="E5">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>43831</v>
       </c>
@@ -719,13 +816,17 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>-4.2</v>
+        <f t="shared" si="0"/>
+        <v>-4.6242774566473948</v>
       </c>
       <c r="D6">
-        <v>232.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>231</v>
+      </c>
+      <c r="E6">
+        <v>242.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>43831</v>
       </c>
@@ -733,13 +834,17 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>-7.4</v>
+        <f t="shared" si="0"/>
+        <v>-8.9395267309377644</v>
       </c>
       <c r="D7">
-        <v>415.3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>415.6</v>
+      </c>
+      <c r="E7">
+        <v>456.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>43831</v>
       </c>
@@ -747,13 +852,17 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>-7.5</v>
+        <f t="shared" si="0"/>
+        <v>-9.9502487562189046</v>
       </c>
       <c r="D8">
-        <v>35.700000000000003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="E8">
+        <v>40.200000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>43831</v>
       </c>
@@ -761,13 +870,17 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>9.4</v>
+        <f t="shared" si="0"/>
+        <v>9.0909090909090953</v>
       </c>
       <c r="D9">
-        <v>37.299999999999997</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="E9">
+        <v>34.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>43831</v>
       </c>
@@ -775,13 +888,17 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>8.9221556886227589</v>
       </c>
       <c r="D10">
-        <v>181.7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>181.9</v>
+      </c>
+      <c r="E10">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>43831</v>
       </c>
@@ -789,27 +906,35 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>-5.2</v>
+        <f t="shared" si="0"/>
+        <v>-4.2505592841163233</v>
       </c>
       <c r="D11">
-        <v>118.8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>128.4</v>
+      </c>
+      <c r="E11">
+        <v>134.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="2">
         <v>43862</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="3">
-        <v>-1.9</v>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>-1.8633540372670849</v>
       </c>
       <c r="D12" s="3">
-        <v>30.3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>31.6</v>
+      </c>
+      <c r="E12">
+        <v>32.200000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>43862</v>
       </c>
@@ -817,13 +942,17 @@
         <v>5</v>
       </c>
       <c r="C13">
-        <v>-16.7</v>
+        <f t="shared" si="0"/>
+        <v>-16.470588235294123</v>
       </c>
       <c r="D13">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>7.1</v>
+      </c>
+      <c r="E13">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>43862</v>
       </c>
@@ -831,13 +960,17 @@
         <v>6</v>
       </c>
       <c r="C14">
-        <v>24.8</v>
+        <f t="shared" si="0"/>
+        <v>23.404255319148945</v>
       </c>
       <c r="D14">
-        <v>39.799999999999997</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>40.6</v>
+      </c>
+      <c r="E14">
+        <v>32.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>43862</v>
       </c>
@@ -845,13 +978,17 @@
         <v>7</v>
       </c>
       <c r="C15">
-        <v>-17.5</v>
+        <f t="shared" si="0"/>
+        <v>-16.860465116279062</v>
       </c>
       <c r="D15">
-        <v>26.9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>28.6</v>
+      </c>
+      <c r="E15">
+        <v>34.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>43862</v>
       </c>
@@ -859,13 +996,17 @@
         <v>8</v>
       </c>
       <c r="C16">
-        <v>-13.8</v>
+        <f t="shared" si="0"/>
+        <v>-17.032520325203254</v>
       </c>
       <c r="D16">
-        <v>204.7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>204.1</v>
+      </c>
+      <c r="E16">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>43862</v>
       </c>
@@ -873,13 +1014,17 @@
         <v>9</v>
       </c>
       <c r="C17">
-        <v>-1.6</v>
+        <f t="shared" si="0"/>
+        <v>-2.4674742036787798</v>
       </c>
       <c r="D17">
-        <v>436.4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>434.8</v>
+      </c>
+      <c r="E17">
+        <v>445.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>43862</v>
       </c>
@@ -887,13 +1032,17 @@
         <v>10</v>
       </c>
       <c r="C18">
-        <v>-2.2000000000000002</v>
+        <f t="shared" si="0"/>
+        <v>-3.49462365591399</v>
       </c>
       <c r="D18">
-        <v>35.299999999999997</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>35.9</v>
+      </c>
+      <c r="E18">
+        <v>37.200000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1">
         <v>43862</v>
       </c>
@@ -901,13 +1050,17 @@
         <v>11</v>
       </c>
       <c r="C19">
-        <v>8.5</v>
+        <f t="shared" si="0"/>
+        <v>9.6866096866096818</v>
       </c>
       <c r="D19">
-        <v>38.299999999999997</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>38.5</v>
+      </c>
+      <c r="E19">
+        <v>35.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>43862</v>
       </c>
@@ -915,13 +1068,17 @@
         <v>12</v>
       </c>
       <c r="C20">
-        <v>-0.8</v>
+        <f t="shared" si="0"/>
+        <v>2.1812080536912624</v>
       </c>
       <c r="D20">
-        <v>180.3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>182.7</v>
+      </c>
+      <c r="E20">
+        <v>178.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1">
         <v>43862</v>
       </c>
@@ -929,27 +1086,35 @@
         <v>13</v>
       </c>
       <c r="C21">
-        <v>10.6</v>
+        <f t="shared" si="0"/>
+        <v>12.440570522979399</v>
       </c>
       <c r="D21">
-        <v>134.69999999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>141.9</v>
+      </c>
+      <c r="E21">
+        <v>126.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="2">
         <v>43891</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="3">
-        <v>-4.3</v>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>-9.177215189873424</v>
       </c>
       <c r="D22" s="3">
-        <v>28.9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>28.7</v>
+      </c>
+      <c r="E22">
+        <v>31.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="1">
         <v>43891</v>
       </c>
@@ -957,13 +1122,17 @@
         <v>5</v>
       </c>
       <c r="C23">
-        <v>-1.3</v>
+        <f t="shared" si="0"/>
+        <v>1.3157894736842175</v>
       </c>
       <c r="D23">
-        <v>7.4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>7.7</v>
+      </c>
+      <c r="E23">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="1">
         <v>43891</v>
       </c>
@@ -971,13 +1140,17 @@
         <v>6</v>
       </c>
       <c r="C24">
-        <v>42.7</v>
+        <f t="shared" si="0"/>
+        <v>43.124999999999993</v>
       </c>
       <c r="D24">
-        <v>44.1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>45.8</v>
+      </c>
+      <c r="E24">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="1">
         <v>43891</v>
       </c>
@@ -985,13 +1158,17 @@
         <v>7</v>
       </c>
       <c r="C25">
-        <v>8.8000000000000007</v>
+        <f t="shared" si="0"/>
+        <v>10.126582278480999</v>
       </c>
       <c r="D25">
-        <v>33.299999999999997</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="E25">
+        <v>31.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="1">
         <v>43891</v>
       </c>
@@ -999,13 +1176,17 @@
         <v>8</v>
       </c>
       <c r="C26">
-        <v>54.7</v>
+        <f t="shared" si="0"/>
+        <v>52.997903563941293</v>
       </c>
       <c r="D26">
-        <v>362.8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>364.9</v>
+      </c>
+      <c r="E26">
+        <v>238.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="1">
         <v>43891</v>
       </c>
@@ -1013,13 +1194,17 @@
         <v>9</v>
       </c>
       <c r="C27">
-        <v>27.5</v>
+        <f t="shared" si="0"/>
+        <v>23.378027681660907</v>
       </c>
       <c r="D27">
-        <v>585.6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>570.5</v>
+      </c>
+      <c r="E27">
+        <v>462.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="1">
         <v>43891</v>
       </c>
@@ -1027,13 +1212,17 @@
         <v>10</v>
       </c>
       <c r="C28">
-        <v>26.9</v>
+        <f t="shared" si="0"/>
+        <v>27.374301675977669</v>
       </c>
       <c r="D28">
-        <v>43.9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>45.6</v>
+      </c>
+      <c r="E28">
+        <v>35.799999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="1">
         <v>43891</v>
       </c>
@@ -1041,13 +1230,17 @@
         <v>11</v>
       </c>
       <c r="C29">
-        <v>43.1</v>
+        <f t="shared" si="0"/>
+        <v>44.44444444444445</v>
       </c>
       <c r="D29">
-        <v>43.8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+        <v>44.2</v>
+      </c>
+      <c r="E29">
+        <v>30.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="1">
         <v>43891</v>
       </c>
@@ -1055,13 +1248,17 @@
         <v>12</v>
       </c>
       <c r="C30">
-        <v>22.7</v>
+        <f t="shared" si="0"/>
+        <v>30.437387657279796</v>
       </c>
       <c r="D30">
-        <v>210.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>217.7</v>
+      </c>
+      <c r="E30">
+        <v>166.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="1">
         <v>43891</v>
       </c>
@@ -1069,13 +1266,17 @@
         <v>13</v>
       </c>
       <c r="C31">
-        <v>48.3</v>
+        <f t="shared" si="0"/>
+        <v>46.712018140589549</v>
       </c>
       <c r="D31">
-        <v>186.7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>194.1</v>
+      </c>
+      <c r="E31">
+        <v>132.30000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="1">
         <v>43922</v>
       </c>
@@ -1083,13 +1284,17 @@
         <v>14</v>
       </c>
       <c r="C32">
-        <v>17</v>
+        <f t="shared" si="0"/>
+        <v>14.241486068111461</v>
       </c>
       <c r="D32">
-        <v>35.799999999999997</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>36.9</v>
+      </c>
+      <c r="E32">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="1">
         <v>43922</v>
       </c>
@@ -1097,13 +1302,17 @@
         <v>5</v>
       </c>
       <c r="C33">
-        <v>15.1</v>
+        <f t="shared" si="0"/>
+        <v>13.333333333333334</v>
       </c>
       <c r="D33">
-        <v>8.4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>8.5</v>
+      </c>
+      <c r="E33">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="1">
         <v>43922</v>
       </c>
@@ -1111,13 +1320,17 @@
         <v>6</v>
       </c>
       <c r="C34">
-        <v>55.6</v>
+        <f t="shared" si="0"/>
+        <v>59.248554913294797</v>
       </c>
       <c r="D34">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+        <v>55.1</v>
+      </c>
+      <c r="E34">
+        <v>34.6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="1">
         <v>43922</v>
       </c>
@@ -1125,13 +1338,17 @@
         <v>7</v>
       </c>
       <c r="C35">
-        <v>52.8</v>
+        <f t="shared" si="0"/>
+        <v>49.535603715170282</v>
       </c>
       <c r="D35">
-        <v>47.2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+        <v>48.3</v>
+      </c>
+      <c r="E35">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="1">
         <v>43922</v>
       </c>
@@ -1139,13 +1356,17 @@
         <v>8</v>
       </c>
       <c r="C36">
-        <v>224.2</v>
+        <f t="shared" si="0"/>
+        <v>234.51327433628316</v>
       </c>
       <c r="D36">
-        <v>729.4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+        <v>756</v>
+      </c>
+      <c r="E36">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="1">
         <v>43922</v>
       </c>
@@ -1153,13 +1374,17 @@
         <v>9</v>
       </c>
       <c r="C37">
-        <v>76.900000000000006</v>
+        <f t="shared" si="0"/>
+        <v>73.378839590443661</v>
       </c>
       <c r="D37">
-        <v>822.4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+        <v>812.8</v>
+      </c>
+      <c r="E37">
+        <v>468.8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="1">
         <v>43922</v>
       </c>
@@ -1167,13 +1392,17 @@
         <v>10</v>
       </c>
       <c r="C38">
-        <v>107.6</v>
+        <f t="shared" si="0"/>
+        <v>100.55096418732784</v>
       </c>
       <c r="D38">
-        <v>73.7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+        <v>72.8</v>
+      </c>
+      <c r="E38">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="1">
         <v>43922</v>
       </c>
@@ -1181,13 +1410,17 @@
         <v>11</v>
       </c>
       <c r="C39">
-        <v>92.6</v>
+        <f t="shared" si="0"/>
+        <v>85.38011695906431</v>
       </c>
       <c r="D39">
-        <v>64.7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+        <v>63.4</v>
+      </c>
+      <c r="E39">
+        <v>34.200000000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="1">
         <v>43922</v>
       </c>
@@ -1195,13 +1428,17 @@
         <v>12</v>
       </c>
       <c r="C40">
-        <v>80.599999999999994</v>
+        <f t="shared" si="0"/>
+        <v>82.055961070559619</v>
       </c>
       <c r="D40">
-        <v>304.3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+        <v>299.3</v>
+      </c>
+      <c r="E40">
+        <v>164.4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="1">
         <v>43922</v>
       </c>
@@ -1209,13 +1446,17 @@
         <v>13</v>
       </c>
       <c r="C41">
-        <v>125.1</v>
+        <f t="shared" si="0"/>
+        <v>122.91187739463601</v>
       </c>
       <c r="D41">
-        <v>278.39999999999998</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>290.89999999999998</v>
+      </c>
+      <c r="E41">
+        <v>130.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="1">
         <v>43952</v>
       </c>
@@ -1223,13 +1464,17 @@
         <v>14</v>
       </c>
       <c r="C42">
-        <v>20.2</v>
+        <f t="shared" si="0"/>
+        <v>25.227963525835879</v>
       </c>
       <c r="D42">
-        <v>38.700000000000003</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>41.2</v>
+      </c>
+      <c r="E42">
+        <v>32.9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="1">
         <v>43952</v>
       </c>
@@ -1237,13 +1482,17 @@
         <v>5</v>
       </c>
       <c r="C43">
-        <v>52.6</v>
+        <f t="shared" si="0"/>
+        <v>56.578947368421062</v>
       </c>
       <c r="D43">
-        <v>11.6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+        <v>11.9</v>
+      </c>
+      <c r="E43">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="1">
         <v>43952</v>
       </c>
@@ -1251,13 +1500,17 @@
         <v>6</v>
       </c>
       <c r="C44">
-        <v>89.3</v>
+        <f t="shared" si="0"/>
+        <v>89.090909090909093</v>
       </c>
       <c r="D44">
-        <v>63.4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>62.4</v>
+      </c>
+      <c r="E44">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="1">
         <v>43952</v>
       </c>
@@ -1265,13 +1518,17 @@
         <v>7</v>
       </c>
       <c r="C45">
-        <v>68.5</v>
+        <f t="shared" si="0"/>
+        <v>69.696969696969703</v>
       </c>
       <c r="D45">
-        <v>48.2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <v>50.4</v>
+      </c>
+      <c r="E45">
+        <v>29.7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" s="1">
         <v>43952</v>
       </c>
@@ -1279,13 +1536,17 @@
         <v>8</v>
       </c>
       <c r="C46">
-        <v>166.5</v>
+        <f t="shared" si="0"/>
+        <v>163.3303808680248</v>
       </c>
       <c r="D46">
-        <v>603.9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+        <v>594.6</v>
+      </c>
+      <c r="E46">
+        <v>225.8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="1">
         <v>43952</v>
       </c>
@@ -1293,13 +1554,17 @@
         <v>9</v>
       </c>
       <c r="C47">
-        <v>145.19999999999999</v>
+        <f t="shared" si="0"/>
+        <v>141.62609542356378</v>
       </c>
       <c r="D47">
-        <v>1003.4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+        <v>992.6</v>
+      </c>
+      <c r="E47">
+        <v>410.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="1">
         <v>43952</v>
       </c>
@@ -1307,13 +1572,17 @@
         <v>10</v>
       </c>
       <c r="C48">
-        <v>112</v>
+        <f t="shared" si="0"/>
+        <v>112.9943502824859</v>
       </c>
       <c r="D48">
-        <v>74.400000000000006</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="E48">
+        <v>35.4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" s="1">
         <v>43952</v>
       </c>
@@ -1321,13 +1590,17 @@
         <v>11</v>
       </c>
       <c r="C49">
-        <v>125.5</v>
+        <f t="shared" si="0"/>
+        <v>120.43343653250777</v>
       </c>
       <c r="D49">
-        <v>72.400000000000006</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>71.2</v>
+      </c>
+      <c r="E49">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" s="1">
         <v>43952</v>
       </c>
@@ -1335,13 +1608,17 @@
         <v>12</v>
       </c>
       <c r="C50">
-        <v>116</v>
+        <f t="shared" si="0"/>
+        <v>117.82238442822386</v>
       </c>
       <c r="D50">
-        <v>365.1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+        <v>358.1</v>
+      </c>
+      <c r="E50">
+        <v>164.4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="1">
         <v>43952</v>
       </c>
@@ -1349,13 +1626,17 @@
         <v>13</v>
       </c>
       <c r="C51">
-        <v>185.3</v>
+        <f t="shared" si="0"/>
+        <v>189.23582580115038</v>
       </c>
       <c r="D51">
-        <v>338.1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>352</v>
+      </c>
+      <c r="E51">
+        <v>121.7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" s="1">
         <v>43983</v>
       </c>
@@ -1363,13 +1644,17 @@
         <v>14</v>
       </c>
       <c r="C52">
-        <v>18.600000000000001</v>
+        <f t="shared" si="0"/>
+        <v>28.613569321533934</v>
       </c>
       <c r="D52">
-        <v>40.200000000000003</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+        <v>43.6</v>
+      </c>
+      <c r="E52">
+        <v>33.9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" s="1">
         <v>43983</v>
       </c>
@@ -1377,13 +1662,17 @@
         <v>5</v>
       </c>
       <c r="C53">
-        <v>69.2</v>
+        <f t="shared" si="0"/>
+        <v>75.999999999999986</v>
       </c>
       <c r="D53">
         <v>13.2</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="E53">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" s="1">
         <v>43983</v>
       </c>
@@ -1391,13 +1680,17 @@
         <v>6</v>
       </c>
       <c r="C54">
-        <v>91.1</v>
+        <f t="shared" si="0"/>
+        <v>90.434782608695656</v>
       </c>
       <c r="D54">
-        <v>64.599999999999994</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
+        <v>65.7</v>
+      </c>
+      <c r="E54">
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" s="1">
         <v>43983</v>
       </c>
@@ -1405,13 +1698,17 @@
         <v>7</v>
       </c>
       <c r="C55">
-        <v>25.6</v>
+        <f t="shared" si="0"/>
+        <v>26.006191950464412</v>
       </c>
       <c r="D55">
-        <v>38.700000000000003</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="E55">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" s="1">
         <v>43983</v>
       </c>
@@ -1419,13 +1716,17 @@
         <v>8</v>
       </c>
       <c r="C56">
-        <v>116.4</v>
+        <f t="shared" si="0"/>
+        <v>114.75189986589183</v>
       </c>
       <c r="D56">
-        <v>485.3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
+        <v>480.4</v>
+      </c>
+      <c r="E56">
+        <v>223.7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" s="1">
         <v>43983</v>
       </c>
@@ -1433,13 +1734,17 @@
         <v>9</v>
       </c>
       <c r="C57">
-        <v>119</v>
+        <f t="shared" si="0"/>
+        <v>116.53197875779264</v>
       </c>
       <c r="D57">
-        <v>943.3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
+        <v>937.8</v>
+      </c>
+      <c r="E57">
+        <v>433.1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" s="1">
         <v>43983</v>
       </c>
@@ -1447,13 +1752,17 @@
         <v>10</v>
       </c>
       <c r="C58">
-        <v>77.2</v>
+        <f t="shared" si="0"/>
+        <v>82.307692307692292</v>
       </c>
       <c r="D58">
-        <v>69.099999999999994</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="E58">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" s="1">
         <v>43983</v>
       </c>
@@ -1461,13 +1770,17 @@
         <v>11</v>
       </c>
       <c r="C59">
-        <v>121.8</v>
+        <f t="shared" si="0"/>
+        <v>120.95238095238095</v>
       </c>
       <c r="D59">
-        <v>70.3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="E59">
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" s="1">
         <v>43983</v>
       </c>
@@ -1475,13 +1788,17 @@
         <v>12</v>
       </c>
       <c r="C60">
-        <v>127.9</v>
+        <f t="shared" si="0"/>
+        <v>132.00241984271022</v>
       </c>
       <c r="D60">
-        <v>382.5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
+        <v>383.5</v>
+      </c>
+      <c r="E60">
+        <v>165.3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61" s="1">
         <v>43983</v>
       </c>
@@ -1489,13 +1806,17 @@
         <v>13</v>
       </c>
       <c r="C61">
-        <v>180.9</v>
+        <f t="shared" si="0"/>
+        <v>192.23454833597467</v>
       </c>
       <c r="D61">
-        <v>345.5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
+        <v>368.8</v>
+      </c>
+      <c r="E61">
+        <v>126.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62" s="1">
         <v>44013</v>
       </c>
@@ -1503,13 +1824,17 @@
         <v>14</v>
       </c>
       <c r="C62">
-        <v>18.399999999999999</v>
+        <f t="shared" si="0"/>
+        <v>24.159021406727824</v>
       </c>
       <c r="D62">
-        <v>38.6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
+        <v>40.6</v>
+      </c>
+      <c r="E62">
+        <v>32.700000000000003</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63" s="1">
         <v>44013</v>
       </c>
@@ -1517,13 +1842,17 @@
         <v>5</v>
       </c>
       <c r="C63">
-        <v>37.5</v>
+        <f t="shared" si="0"/>
+        <v>42.857142857142854</v>
       </c>
       <c r="D63">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
+        <v>10</v>
+      </c>
+      <c r="E63">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64" s="1">
         <v>44013</v>
       </c>
@@ -1531,13 +1860,17 @@
         <v>6</v>
       </c>
       <c r="C64">
-        <v>41.6</v>
+        <f t="shared" si="0"/>
+        <v>40.750670241286876</v>
       </c>
       <c r="D64">
-        <v>52.8</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
+        <v>52.5</v>
+      </c>
+      <c r="E64">
+        <v>37.299999999999997</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65" s="1">
         <v>44013</v>
       </c>
@@ -1545,13 +1878,17 @@
         <v>7</v>
       </c>
       <c r="C65">
-        <v>15.2</v>
+        <f t="shared" si="0"/>
+        <v>15.835777126099702</v>
       </c>
       <c r="D65">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
+        <v>39.5</v>
+      </c>
+      <c r="E65">
+        <v>34.1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66" s="1">
         <v>44013</v>
       </c>
@@ -1559,13 +1896,17 @@
         <v>8</v>
       </c>
       <c r="C66">
-        <v>94.7</v>
+        <f t="shared" si="0"/>
+        <v>87.39569609134827</v>
       </c>
       <c r="D66">
-        <v>436.8</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
+        <v>426.7</v>
+      </c>
+      <c r="E66">
+        <v>227.7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67" s="1">
         <v>44013</v>
       </c>
@@ -1573,13 +1914,17 @@
         <v>9</v>
       </c>
       <c r="C67">
-        <v>98.2</v>
+        <f t="shared" si="0"/>
+        <v>95.125751168484314</v>
       </c>
       <c r="D67">
-        <v>886.6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
+        <v>876.7</v>
+      </c>
+      <c r="E67">
+        <v>449.3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68" s="1">
         <v>44013</v>
       </c>
@@ -1587,13 +1932,17 @@
         <v>10</v>
       </c>
       <c r="C68">
-        <v>41.5</v>
+        <f t="shared" ref="C68:C131" si="1">(D68-E68)/E68*100</f>
+        <v>48.120300751879711</v>
       </c>
       <c r="D68">
-        <v>56.3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
+        <v>59.1</v>
+      </c>
+      <c r="E68">
+        <v>39.9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69" s="1">
         <v>44013</v>
       </c>
@@ -1601,13 +1950,17 @@
         <v>11</v>
       </c>
       <c r="C69">
-        <v>59.9</v>
+        <f t="shared" si="1"/>
+        <v>58.997050147492622</v>
       </c>
       <c r="D69">
-        <v>53.1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
+        <v>53.9</v>
+      </c>
+      <c r="E69">
+        <v>33.9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70" s="1">
         <v>44013</v>
       </c>
@@ -1615,13 +1968,17 @@
         <v>12</v>
       </c>
       <c r="C70">
-        <v>77.2</v>
+        <f t="shared" si="1"/>
+        <v>75.364758698092032</v>
       </c>
       <c r="D70">
-        <v>316.10000000000002</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
+        <v>312.5</v>
+      </c>
+      <c r="E70">
+        <v>178.2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71" s="1">
         <v>44013</v>
       </c>
@@ -1629,13 +1986,17 @@
         <v>13</v>
       </c>
       <c r="C71">
-        <v>145.9</v>
+        <f t="shared" si="1"/>
+        <v>148.44373503591382</v>
       </c>
       <c r="D71">
-        <v>295.3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
+        <v>311.3</v>
+      </c>
+      <c r="E71">
+        <v>125.3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72" s="1">
         <v>44044</v>
       </c>
@@ -1643,13 +2004,17 @@
         <v>14</v>
       </c>
       <c r="C72">
-        <v>-3.6</v>
+        <f t="shared" si="1"/>
+        <v>-3.9156626506024224</v>
       </c>
       <c r="D72">
-        <v>32.1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
+        <v>31.9</v>
+      </c>
+      <c r="E72">
+        <v>33.200000000000003</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73" s="1">
         <v>44044</v>
       </c>
@@ -1657,13 +2022,17 @@
         <v>5</v>
       </c>
       <c r="C73">
-        <v>19.7</v>
+        <f t="shared" si="1"/>
+        <v>24.000000000000011</v>
       </c>
       <c r="D73">
-        <v>9.1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="E73">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74" s="1">
         <v>44044</v>
       </c>
@@ -1671,13 +2040,17 @@
         <v>6</v>
       </c>
       <c r="C74">
-        <v>27.3</v>
+        <f t="shared" si="1"/>
+        <v>24.504950495049503</v>
       </c>
       <c r="D74">
-        <v>50.8</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
+        <v>50.3</v>
+      </c>
+      <c r="E74">
+        <v>40.4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
       <c r="A75" s="1">
         <v>44044</v>
       </c>
@@ -1685,13 +2058,17 @@
         <v>7</v>
       </c>
       <c r="C75">
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>7.5801749271137071</v>
       </c>
       <c r="D75">
-        <v>36.200000000000003</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
+        <v>36.9</v>
+      </c>
+      <c r="E75">
+        <v>34.299999999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
       <c r="A76" s="1">
         <v>44044</v>
       </c>
@@ -1699,13 +2076,17 @@
         <v>8</v>
       </c>
       <c r="C76">
-        <v>83.6</v>
+        <f t="shared" si="1"/>
+        <v>79.336620349619025</v>
       </c>
       <c r="D76">
-        <v>398.4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
+        <v>400.1</v>
+      </c>
+      <c r="E76">
+        <v>223.1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77" s="1">
         <v>44044</v>
       </c>
@@ -1713,13 +2094,17 @@
         <v>9</v>
       </c>
       <c r="C77">
-        <v>90</v>
+        <f t="shared" si="1"/>
+        <v>86.363636363636388</v>
       </c>
       <c r="D77">
-        <v>841.4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
+        <v>828.2</v>
+      </c>
+      <c r="E77">
+        <v>444.4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78" s="1">
         <v>44044</v>
       </c>
@@ -1727,13 +2112,17 @@
         <v>10</v>
       </c>
       <c r="C78">
-        <v>45.8</v>
+        <f t="shared" si="1"/>
+        <v>51.978891820580486</v>
       </c>
       <c r="D78">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
+        <v>57.6</v>
+      </c>
+      <c r="E78">
+        <v>37.9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79" s="1">
         <v>44044</v>
       </c>
@@ -1741,13 +2130,17 @@
         <v>11</v>
       </c>
       <c r="C79">
-        <v>53.9</v>
+        <f t="shared" si="1"/>
+        <v>46.708463949843257</v>
       </c>
       <c r="D79">
-        <v>47.7</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
+        <v>46.8</v>
+      </c>
+      <c r="E79">
+        <v>31.9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80" s="1">
         <v>44044</v>
       </c>
@@ -1755,13 +2148,17 @@
         <v>12</v>
       </c>
       <c r="C80">
-        <v>59.2</v>
+        <f t="shared" si="1"/>
+        <v>62.5548245614035</v>
       </c>
       <c r="D80">
-        <v>290.39999999999998</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
+        <v>296.5</v>
+      </c>
+      <c r="E80">
+        <v>182.4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" s="1">
         <v>44044</v>
       </c>
@@ -1769,13 +2166,17 @@
         <v>13</v>
       </c>
       <c r="C81">
-        <v>112.5</v>
+        <f t="shared" si="1"/>
+        <v>110.03533568904594</v>
       </c>
       <c r="D81">
-        <v>284.89999999999998</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
+        <v>297.2</v>
+      </c>
+      <c r="E81">
+        <v>141.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82" s="1">
         <v>44075</v>
       </c>
@@ -1783,13 +2184,17 @@
         <v>14</v>
       </c>
       <c r="C82">
-        <v>30.9</v>
+        <f t="shared" si="1"/>
+        <v>32.094594594594597</v>
       </c>
       <c r="D82">
-        <v>37.700000000000003</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
+        <v>39.1</v>
+      </c>
+      <c r="E82">
+        <v>29.6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83" s="1">
         <v>44075</v>
       </c>
@@ -1797,13 +2202,17 @@
         <v>5</v>
       </c>
       <c r="C83">
-        <v>14.9</v>
+        <f t="shared" si="1"/>
+        <v>17.80821917808219</v>
       </c>
       <c r="D83">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
+        <v>8.6</v>
+      </c>
+      <c r="E83">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" s="1">
         <v>44075</v>
       </c>
@@ -1811,13 +2220,17 @@
         <v>6</v>
       </c>
       <c r="C84">
-        <v>6.9</v>
+        <f t="shared" si="1"/>
+        <v>7.3170731707317156</v>
       </c>
       <c r="D84">
-        <v>38.9</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
+        <v>39.6</v>
+      </c>
+      <c r="E84">
+        <v>36.9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" s="1">
         <v>44075</v>
       </c>
@@ -1825,13 +2238,17 @@
         <v>7</v>
       </c>
       <c r="C85">
-        <v>28.9</v>
+        <f t="shared" si="1"/>
+        <v>35.714285714285708</v>
       </c>
       <c r="D85">
-        <v>40.6</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
+        <v>43.7</v>
+      </c>
+      <c r="E85">
+        <v>32.200000000000003</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86" s="1">
         <v>44075</v>
       </c>
@@ -1839,13 +2256,17 @@
         <v>8</v>
       </c>
       <c r="C86">
-        <v>52.2</v>
+        <f t="shared" si="1"/>
+        <v>47.83923941227313</v>
       </c>
       <c r="D86">
-        <v>341.9</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4">
+        <v>342.1</v>
+      </c>
+      <c r="E86">
+        <v>231.4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87" s="1">
         <v>44075</v>
       </c>
@@ -1853,13 +2274,17 @@
         <v>9</v>
       </c>
       <c r="C87">
-        <v>80.2</v>
+        <f t="shared" si="1"/>
+        <v>80.776560266793695</v>
       </c>
       <c r="D87">
-        <v>757.4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
+        <v>758.9</v>
+      </c>
+      <c r="E87">
+        <v>419.8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88" s="1">
         <v>44075</v>
       </c>
@@ -1867,13 +2292,17 @@
         <v>10</v>
       </c>
       <c r="C88">
+        <f t="shared" si="1"/>
+        <v>47.774480712166152</v>
+      </c>
+      <c r="D88">
         <v>49.8</v>
       </c>
-      <c r="D88">
-        <v>49.3</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
+      <c r="E88">
+        <v>33.700000000000003</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89" s="1">
         <v>44075</v>
       </c>
@@ -1881,13 +2310,17 @@
         <v>11</v>
       </c>
       <c r="C89">
-        <v>26.6</v>
+        <f t="shared" si="1"/>
+        <v>27.027027027027028</v>
       </c>
       <c r="D89">
-        <v>41.4</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
+        <v>42.3</v>
+      </c>
+      <c r="E89">
+        <v>33.299999999999997</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90" s="1">
         <v>44075</v>
       </c>
@@ -1895,13 +2328,17 @@
         <v>12</v>
       </c>
       <c r="C90">
-        <v>77.7</v>
+        <f t="shared" si="1"/>
+        <v>80.65693430656934</v>
       </c>
       <c r="D90">
-        <v>293.2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4">
+        <v>297</v>
+      </c>
+      <c r="E90">
+        <v>164.4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91" s="1">
         <v>44075</v>
       </c>
@@ -1909,13 +2346,17 @@
         <v>13</v>
       </c>
       <c r="C91">
-        <v>73.7</v>
+        <f t="shared" si="1"/>
+        <v>74.668630338733408</v>
       </c>
       <c r="D91">
-        <v>223.7</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
+        <v>237.2</v>
+      </c>
+      <c r="E91">
+        <v>135.80000000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92" s="1">
         <v>44105</v>
       </c>
@@ -1923,13 +2364,17 @@
         <v>14</v>
       </c>
       <c r="C92">
-        <v>15.5</v>
+        <f t="shared" si="1"/>
+        <v>12.04013377926422</v>
       </c>
       <c r="D92">
-        <v>32.700000000000003</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
+        <v>33.5</v>
+      </c>
+      <c r="E92">
+        <v>29.9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93" s="1">
         <v>44105</v>
       </c>
@@ -1937,13 +2382,17 @@
         <v>5</v>
       </c>
       <c r="C93">
-        <v>19.7</v>
+        <f t="shared" si="1"/>
+        <v>23.287671232876718</v>
       </c>
       <c r="D93">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4">
+        <v>9</v>
+      </c>
+      <c r="E93">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94" s="1">
         <v>44105</v>
       </c>
@@ -1951,13 +2400,17 @@
         <v>6</v>
       </c>
       <c r="C94">
-        <v>6.6</v>
+        <f t="shared" si="1"/>
+        <v>7.9710144927536337</v>
       </c>
       <c r="D94">
-        <v>43.8</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
+        <v>44.7</v>
+      </c>
+      <c r="E94">
+        <v>41.4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95" s="1">
         <v>44105</v>
       </c>
@@ -1965,13 +2418,17 @@
         <v>7</v>
       </c>
       <c r="C95">
-        <v>27.3</v>
+        <f t="shared" si="1"/>
+        <v>30.817610062893085</v>
       </c>
       <c r="D95">
-        <v>39.6</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4">
+        <v>41.6</v>
+      </c>
+      <c r="E95">
+        <v>31.8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
       <c r="A96" s="1">
         <v>44105</v>
       </c>
@@ -1979,13 +2436,17 @@
         <v>8</v>
       </c>
       <c r="C96">
-        <v>53.3</v>
+        <f t="shared" si="1"/>
+        <v>50.512820512820511</v>
       </c>
       <c r="D96">
-        <v>354.2</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
+        <v>352.2</v>
+      </c>
+      <c r="E96">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97" s="1">
         <v>44105</v>
       </c>
@@ -1993,13 +2454,17 @@
         <v>9</v>
       </c>
       <c r="C97">
-        <v>81.3</v>
+        <f t="shared" si="1"/>
+        <v>82.828760643330185</v>
       </c>
       <c r="D97">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
+        <v>773</v>
+      </c>
+      <c r="E97">
+        <v>422.8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98" s="1">
         <v>44105</v>
       </c>
@@ -2007,13 +2472,17 @@
         <v>10</v>
       </c>
       <c r="C98">
-        <v>36.5</v>
+        <f t="shared" si="1"/>
+        <v>34.604904632152575</v>
       </c>
       <c r="D98">
-        <v>49.7</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4">
+        <v>49.4</v>
+      </c>
+      <c r="E98">
+        <v>36.700000000000003</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
       <c r="A99" s="1">
         <v>44105</v>
       </c>
@@ -2021,13 +2490,17 @@
         <v>11</v>
       </c>
       <c r="C99">
-        <v>20.100000000000001</v>
+        <f t="shared" si="1"/>
+        <v>24.299065420560737</v>
       </c>
       <c r="D99">
-        <v>38.200000000000003</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4">
+        <v>39.9</v>
+      </c>
+      <c r="E99">
+        <v>32.1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
       <c r="A100" s="1">
         <v>44105</v>
       </c>
@@ -2035,13 +2508,17 @@
         <v>12</v>
       </c>
       <c r="C100">
-        <v>56.7</v>
+        <f t="shared" si="1"/>
+        <v>57.847800237812145</v>
       </c>
       <c r="D100">
-        <v>267.10000000000002</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4">
+        <v>265.5</v>
+      </c>
+      <c r="E100">
+        <v>168.2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
       <c r="A101" s="1">
         <v>44105</v>
       </c>
@@ -2049,13 +2526,17 @@
         <v>13</v>
       </c>
       <c r="C101">
-        <v>67.2</v>
+        <f t="shared" si="1"/>
+        <v>67.287630402384508</v>
       </c>
       <c r="D101">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4">
+        <v>224.5</v>
+      </c>
+      <c r="E101">
+        <v>134.19999999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
       <c r="A102" s="1">
         <v>44136</v>
       </c>
@@ -2063,13 +2544,17 @@
         <v>14</v>
       </c>
       <c r="C102">
-        <v>8.6999999999999993</v>
+        <f t="shared" si="1"/>
+        <v>8.0536912751677914</v>
       </c>
       <c r="D102">
-        <v>31.3</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="E102">
+        <v>29.8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
       <c r="A103" s="1">
         <v>44136</v>
       </c>
@@ -2077,13 +2562,17 @@
         <v>5</v>
       </c>
       <c r="C103">
-        <v>27.5</v>
+        <f t="shared" si="1"/>
+        <v>30.882352941176478</v>
       </c>
       <c r="D103">
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4">
+        <v>8.9</v>
+      </c>
+      <c r="E103">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
       <c r="A104" s="1">
         <v>44136</v>
       </c>
@@ -2091,13 +2580,17 @@
         <v>6</v>
       </c>
       <c r="C104">
-        <v>-19.100000000000001</v>
+        <f t="shared" si="1"/>
+        <v>-17.456359102244388</v>
       </c>
       <c r="D104">
-        <v>32.200000000000003</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4">
+        <v>33.1</v>
+      </c>
+      <c r="E104">
+        <v>40.1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
       <c r="A105" s="1">
         <v>44136</v>
       </c>
@@ -2105,13 +2598,17 @@
         <v>7</v>
       </c>
       <c r="C105">
-        <v>24.4</v>
+        <f t="shared" si="1"/>
+        <v>27.331189710610932</v>
       </c>
       <c r="D105">
-        <v>37.700000000000003</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4">
+        <v>39.6</v>
+      </c>
+      <c r="E105">
+        <v>31.1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
       <c r="A106" s="1">
         <v>44136</v>
       </c>
@@ -2119,13 +2616,17 @@
         <v>8</v>
       </c>
       <c r="C106">
-        <v>29.4</v>
+        <f t="shared" si="1"/>
+        <v>29.066561638440326</v>
       </c>
       <c r="D106">
-        <v>329.7</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4">
+        <v>327.7</v>
+      </c>
+      <c r="E106">
+        <v>253.9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
       <c r="A107" s="1">
         <v>44136</v>
       </c>
@@ -2133,13 +2634,17 @@
         <v>9</v>
       </c>
       <c r="C107">
-        <v>66.599999999999994</v>
+        <f t="shared" si="1"/>
+        <v>68.439226519337041</v>
       </c>
       <c r="D107">
-        <v>733.7</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4">
+        <v>731.7</v>
+      </c>
+      <c r="E107">
+        <v>434.4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
       <c r="A108" s="1">
         <v>44136</v>
       </c>
@@ -2147,13 +2652,17 @@
         <v>10</v>
       </c>
       <c r="C108">
-        <v>32.6</v>
+        <f t="shared" si="1"/>
+        <v>31.876606683804624</v>
       </c>
       <c r="D108">
-        <v>50.9</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4">
+        <v>51.3</v>
+      </c>
+      <c r="E108">
+        <v>38.9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
       <c r="A109" s="1">
         <v>44136</v>
       </c>
@@ -2161,13 +2670,17 @@
         <v>11</v>
       </c>
       <c r="C109">
-        <v>16.5</v>
+        <f t="shared" si="1"/>
+        <v>15.300546448087434</v>
       </c>
       <c r="D109">
-        <v>41.7</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4">
+        <v>42.2</v>
+      </c>
+      <c r="E109">
+        <v>36.6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
       <c r="A110" s="1">
         <v>44136</v>
       </c>
@@ -2175,13 +2688,17 @@
         <v>12</v>
       </c>
       <c r="C110">
-        <v>51.6</v>
+        <f t="shared" si="1"/>
+        <v>49.369171695008227</v>
       </c>
       <c r="D110">
-        <v>276.7</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4">
+        <v>272.3</v>
+      </c>
+      <c r="E110">
+        <v>182.3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
       <c r="A111" s="1">
         <v>44136</v>
       </c>
@@ -2189,13 +2706,17 @@
         <v>13</v>
       </c>
       <c r="C111">
-        <v>43</v>
+        <f t="shared" si="1"/>
+        <v>44.12181303116148</v>
       </c>
       <c r="D111">
-        <v>192.4</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4">
+        <v>203.5</v>
+      </c>
+      <c r="E111">
+        <v>141.19999999999999</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
       <c r="A112" s="1">
         <v>44166</v>
       </c>
@@ -2203,13 +2724,17 @@
         <v>14</v>
       </c>
       <c r="C112">
-        <v>6.1</v>
+        <f t="shared" si="1"/>
+        <v>3.1847133757961785</v>
       </c>
       <c r="D112">
+        <v>32.4</v>
+      </c>
+      <c r="E112">
         <v>31.4</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:5">
       <c r="A113" s="1">
         <v>44166</v>
       </c>
@@ -2217,13 +2742,17 @@
         <v>5</v>
       </c>
       <c r="C113">
-        <v>24.6</v>
+        <f t="shared" si="1"/>
+        <v>25.000000000000007</v>
       </c>
       <c r="D113">
-        <v>8.6</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4">
+        <v>8.5</v>
+      </c>
+      <c r="E113">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
       <c r="A114" s="1">
         <v>44166</v>
       </c>
@@ -2231,13 +2760,17 @@
         <v>6</v>
       </c>
       <c r="C114">
-        <v>9.3000000000000007</v>
+        <f t="shared" si="1"/>
+        <v>8.6848635235732008</v>
       </c>
       <c r="D114">
-        <v>43.4</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4">
+        <v>43.8</v>
+      </c>
+      <c r="E114">
+        <v>40.299999999999997</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
       <c r="A115" s="1">
         <v>44166</v>
       </c>
@@ -2245,13 +2778,17 @@
         <v>7</v>
       </c>
       <c r="C115">
-        <v>26.8</v>
+        <f t="shared" si="1"/>
+        <v>28.619528619528634</v>
       </c>
       <c r="D115">
-        <v>36.4</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="E115">
+        <v>29.7</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
       <c r="A116" s="1">
         <v>44166</v>
       </c>
@@ -2259,13 +2796,17 @@
         <v>8</v>
       </c>
       <c r="C116">
-        <v>26.9</v>
+        <f t="shared" si="1"/>
+        <v>28.559357836924388</v>
       </c>
       <c r="D116">
-        <v>305.8</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4">
+        <v>304.3</v>
+      </c>
+      <c r="E116">
+        <v>236.7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
       <c r="A117" s="1">
         <v>44166</v>
       </c>
@@ -2273,13 +2814,17 @@
         <v>9</v>
       </c>
       <c r="C117">
-        <v>80</v>
+        <f t="shared" si="1"/>
+        <v>84.012389802239682</v>
       </c>
       <c r="D117">
-        <v>762.5</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4">
+        <v>772.3</v>
+      </c>
+      <c r="E117">
+        <v>419.7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
       <c r="A118" s="1">
         <v>44166</v>
       </c>
@@ -2287,13 +2832,17 @@
         <v>10</v>
       </c>
       <c r="C118">
-        <v>61.9</v>
+        <f t="shared" si="1"/>
+        <v>60.398860398860386</v>
       </c>
       <c r="D118">
-        <v>55.7</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4">
+        <v>56.3</v>
+      </c>
+      <c r="E118">
+        <v>35.1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
       <c r="A119" s="1">
         <v>44166</v>
       </c>
@@ -2301,13 +2850,17 @@
         <v>11</v>
       </c>
       <c r="C119">
-        <v>33.5</v>
+        <f t="shared" si="1"/>
+        <v>29.75206611570249</v>
       </c>
       <c r="D119">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4">
+        <v>47.1</v>
+      </c>
+      <c r="E119">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
       <c r="A120" s="1">
         <v>44166</v>
       </c>
@@ -2315,13 +2868,17 @@
         <v>12</v>
       </c>
       <c r="C120">
-        <v>53.9</v>
+        <f t="shared" si="1"/>
+        <v>50.980392156862742</v>
       </c>
       <c r="D120">
-        <v>271.39999999999998</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4">
+        <v>269.5</v>
+      </c>
+      <c r="E120">
+        <v>178.5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
       <c r="A121" s="1">
         <v>44166</v>
       </c>
@@ -2329,13 +2886,17 @@
         <v>13</v>
       </c>
       <c r="C121">
-        <v>51.3</v>
+        <f t="shared" si="1"/>
+        <v>50.186428038777045</v>
       </c>
       <c r="D121">
-        <v>193.7</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4">
+        <v>201.4</v>
+      </c>
+      <c r="E121">
+        <v>134.1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
       <c r="A122" s="1">
         <v>44197</v>
       </c>
@@ -2343,13 +2904,17 @@
         <v>14</v>
       </c>
       <c r="C122">
-        <v>2.8</v>
+        <f t="shared" si="1"/>
+        <v>3.8338658146964835</v>
       </c>
       <c r="D122">
         <v>32.5</v>
       </c>
-    </row>
-    <row r="123" spans="1:4">
+      <c r="E122">
+        <v>31.3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
       <c r="A123" s="1">
         <v>44197</v>
       </c>
@@ -2357,13 +2922,17 @@
         <v>5</v>
       </c>
       <c r="C123">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>-18.292682926829258</v>
       </c>
       <c r="D123">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="124" spans="1:4">
+      <c r="E123">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
       <c r="A124" s="1">
         <v>44197</v>
       </c>
@@ -2371,13 +2940,17 @@
         <v>6</v>
       </c>
       <c r="C124">
-        <v>10.5</v>
+        <f t="shared" si="1"/>
+        <v>19.943019943019944</v>
       </c>
       <c r="D124">
         <v>42.1</v>
       </c>
-    </row>
-    <row r="125" spans="1:4">
+      <c r="E124">
+        <v>35.1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
       <c r="A125" s="1">
         <v>44197</v>
       </c>
@@ -2385,13 +2958,17 @@
         <v>7</v>
       </c>
       <c r="C125">
-        <v>14.5</v>
+        <f t="shared" si="1"/>
+        <v>7.4303405572755592</v>
       </c>
       <c r="D125">
         <v>34.700000000000003</v>
       </c>
-    </row>
-    <row r="126" spans="1:4">
+      <c r="E125">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
       <c r="A126" s="1">
         <v>44197</v>
       </c>
@@ -2399,13 +2976,17 @@
         <v>8</v>
       </c>
       <c r="C126">
-        <v>70.8</v>
+        <f t="shared" si="1"/>
+        <v>62.92320396366641</v>
       </c>
       <c r="D126">
         <v>394.6</v>
       </c>
-    </row>
-    <row r="127" spans="1:4">
+      <c r="E126">
+        <v>242.2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
       <c r="A127" s="1">
         <v>44197</v>
       </c>
@@ -2413,13 +2994,17 @@
         <v>9</v>
       </c>
       <c r="C127">
-        <v>93.1</v>
+        <f t="shared" si="1"/>
+        <v>75.810692375109554</v>
       </c>
       <c r="D127">
         <v>802.4</v>
       </c>
-    </row>
-    <row r="128" spans="1:4">
+      <c r="E127">
+        <v>456.4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
       <c r="A128" s="1">
         <v>44197</v>
       </c>
@@ -2427,13 +3012,17 @@
         <v>10</v>
       </c>
       <c r="C128">
-        <v>51.4</v>
+        <f t="shared" si="1"/>
+        <v>36.318407960198989</v>
       </c>
       <c r="D128">
         <v>54.8</v>
       </c>
-    </row>
-    <row r="129" spans="1:4">
+      <c r="E128">
+        <v>40.200000000000003</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
       <c r="A129" s="1">
         <v>44197</v>
       </c>
@@ -2441,13 +3030,17 @@
         <v>11</v>
       </c>
       <c r="C129">
-        <v>13.7</v>
+        <f t="shared" si="1"/>
+        <v>24.046920821114355</v>
       </c>
       <c r="D129">
         <v>42.3</v>
       </c>
-    </row>
-    <row r="130" spans="1:4">
+      <c r="E129">
+        <v>34.1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
       <c r="A130" s="1">
         <v>44197</v>
       </c>
@@ -2455,13 +3048,17 @@
         <v>12</v>
       </c>
       <c r="C130">
-        <v>44.4</v>
+        <f t="shared" si="1"/>
+        <v>57.305389221556879</v>
       </c>
       <c r="D130">
         <v>262.7</v>
       </c>
-    </row>
-    <row r="131" spans="1:4">
+      <c r="E130">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
       <c r="A131" s="1">
         <v>44197</v>
       </c>
@@ -2469,13 +3066,17 @@
         <v>13</v>
       </c>
       <c r="C131">
-        <v>76.2</v>
+        <f t="shared" si="1"/>
+        <v>68.680089485458609</v>
       </c>
       <c r="D131">
         <v>226.2</v>
       </c>
-    </row>
-    <row r="132" spans="1:4">
+      <c r="E131">
+        <v>134.1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
       <c r="A132" s="1">
         <v>44228</v>
       </c>
@@ -2483,13 +3084,17 @@
         <v>14</v>
       </c>
       <c r="C132">
-        <v>18</v>
+        <f t="shared" ref="C132:C151" si="2">(D132-E132)/E132*100</f>
+        <v>15.838509316770166</v>
       </c>
       <c r="D132">
         <v>37.299999999999997</v>
       </c>
-    </row>
-    <row r="133" spans="1:4">
+      <c r="E132">
+        <v>32.200000000000003</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
       <c r="A133" s="1">
         <v>44228</v>
       </c>
@@ -2497,13 +3102,17 @@
         <v>5</v>
       </c>
       <c r="C133">
-        <v>11.3</v>
+        <f t="shared" si="2"/>
+        <v>-7.0588235294117601</v>
       </c>
       <c r="D133">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="134" spans="1:4">
+      <c r="E133">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
       <c r="A134" s="1">
         <v>44228</v>
       </c>
@@ -2511,13 +3120,17 @@
         <v>6</v>
       </c>
       <c r="C134">
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>24.620060790273563</v>
       </c>
       <c r="D134">
         <v>41</v>
       </c>
-    </row>
-    <row r="135" spans="1:4">
+      <c r="E134">
+        <v>32.9</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
       <c r="A135" s="1">
         <v>44228</v>
       </c>
@@ -2525,13 +3138,17 @@
         <v>7</v>
       </c>
       <c r="C135">
-        <v>22.4</v>
+        <f t="shared" si="2"/>
+        <v>1.7441860465116321</v>
       </c>
       <c r="D135">
         <v>35</v>
       </c>
-    </row>
-    <row r="136" spans="1:4">
+      <c r="E135">
+        <v>34.4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
       <c r="A136" s="1">
         <v>44228</v>
       </c>
@@ -2539,13 +3156,17 @@
         <v>8</v>
       </c>
       <c r="C136">
-        <v>41.8</v>
+        <f t="shared" si="2"/>
+        <v>17.642276422764219</v>
       </c>
       <c r="D136">
         <v>289.39999999999998</v>
       </c>
-    </row>
-    <row r="137" spans="1:4">
+      <c r="E136">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
       <c r="A137" s="1">
         <v>44228</v>
       </c>
@@ -2553,13 +3174,17 @@
         <v>9</v>
       </c>
       <c r="C137">
-        <v>67.099999999999994</v>
+        <f t="shared" si="2"/>
+        <v>62.965455361148493</v>
       </c>
       <c r="D137">
         <v>726.5</v>
       </c>
-    </row>
-    <row r="138" spans="1:4">
+      <c r="E137">
+        <v>445.8</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
       <c r="A138" s="1">
         <v>44228</v>
       </c>
@@ -2567,13 +3192,17 @@
         <v>10</v>
       </c>
       <c r="C138">
-        <v>30.9</v>
+        <f t="shared" si="2"/>
+        <v>26.344086021505365</v>
       </c>
       <c r="D138">
         <v>47</v>
       </c>
-    </row>
-    <row r="139" spans="1:4">
+      <c r="E138">
+        <v>37.200000000000003</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
       <c r="A139" s="1">
         <v>44228</v>
       </c>
@@ -2581,13 +3210,17 @@
         <v>11</v>
       </c>
       <c r="C139">
-        <v>11.9</v>
+        <f t="shared" si="2"/>
+        <v>22.792022792022792</v>
       </c>
       <c r="D139">
         <v>43.1</v>
       </c>
-    </row>
-    <row r="140" spans="1:4">
+      <c r="E139">
+        <v>35.1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
       <c r="A140" s="1">
         <v>44228</v>
       </c>
@@ -2595,13 +3228,17 @@
         <v>12</v>
       </c>
       <c r="C140">
-        <v>32.5</v>
+        <f t="shared" si="2"/>
+        <v>35.402684563758378</v>
       </c>
       <c r="D140">
         <v>242.1</v>
       </c>
-    </row>
-    <row r="141" spans="1:4">
+      <c r="E140">
+        <v>178.8</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
       <c r="A141" s="1">
         <v>44228</v>
       </c>
@@ -2609,10 +3246,194 @@
         <v>13</v>
       </c>
       <c r="C141">
-        <v>38</v>
+        <f t="shared" si="2"/>
+        <v>55.150554675118869</v>
       </c>
       <c r="D141">
         <v>195.8</v>
+      </c>
+      <c r="E141">
+        <v>126.2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C142">
+        <f t="shared" si="2"/>
+        <v>-1.2658227848101333</v>
+      </c>
+      <c r="D142">
+        <v>31.2</v>
+      </c>
+      <c r="E142">
+        <v>31.6</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B143" t="s">
+        <v>5</v>
+      </c>
+      <c r="C143">
+        <f t="shared" si="2"/>
+        <v>-7.8947368421052584</v>
+      </c>
+      <c r="D143">
+        <v>7</v>
+      </c>
+      <c r="E143">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B144" t="s">
+        <v>6</v>
+      </c>
+      <c r="C144">
+        <f t="shared" si="2"/>
+        <v>37.187499999999993</v>
+      </c>
+      <c r="D144">
+        <v>43.9</v>
+      </c>
+      <c r="E144">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B145" t="s">
+        <v>7</v>
+      </c>
+      <c r="C145">
+        <f t="shared" si="2"/>
+        <v>15.822784810126581</v>
+      </c>
+      <c r="D145">
+        <v>36.6</v>
+      </c>
+      <c r="E145">
+        <v>31.6</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B146" t="s">
+        <v>8</v>
+      </c>
+      <c r="C146">
+        <f t="shared" si="2"/>
+        <v>21.299790356394137</v>
+      </c>
+      <c r="D146">
+        <v>289.3</v>
+      </c>
+      <c r="E146">
+        <v>238.5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="A147" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B147" t="s">
+        <v>9</v>
+      </c>
+      <c r="C147">
+        <f t="shared" si="2"/>
+        <v>28.979238754325259</v>
+      </c>
+      <c r="D147">
+        <v>596.4</v>
+      </c>
+      <c r="E147">
+        <v>462.4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B148" t="s">
+        <v>10</v>
+      </c>
+      <c r="C148">
+        <f t="shared" si="2"/>
+        <v>32.402234636871512</v>
+      </c>
+      <c r="D148">
+        <v>47.4</v>
+      </c>
+      <c r="E148">
+        <v>35.799999999999997</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="A149" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B149" t="s">
+        <v>11</v>
+      </c>
+      <c r="C149">
+        <f t="shared" si="2"/>
+        <v>41.830065359477118</v>
+      </c>
+      <c r="D149">
+        <v>43.4</v>
+      </c>
+      <c r="E149">
+        <v>30.6</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
+      <c r="A150" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B150" t="s">
+        <v>12</v>
+      </c>
+      <c r="C150">
+        <f t="shared" si="2"/>
+        <v>33.852606351108449</v>
+      </c>
+      <c r="D150">
+        <v>223.4</v>
+      </c>
+      <c r="E150">
+        <v>166.9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="A151" s="1">
+        <v>44256</v>
+      </c>
+      <c r="B151" t="s">
+        <v>13</v>
+      </c>
+      <c r="C151">
+        <f t="shared" si="2"/>
+        <v>49.735449735449713</v>
+      </c>
+      <c r="D151">
+        <v>198.1</v>
+      </c>
+      <c r="E151">
+        <v>132.30000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data: 7 May 2021
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C16" si="0">(D3-E3)/E3*100</f>
+        <f t="shared" ref="C3:C17" si="0">(D3-E3)/E3*100</f>
         <v>-2.6758409785932722</v>
       </c>
       <c r="D3">
@@ -698,6 +698,24 @@
       </c>
       <c r="E16">
         <v>1169.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>40.569029051332578</v>
+      </c>
+      <c r="D17">
+        <v>1640.3</v>
+      </c>
+      <c r="E17">
+        <v>1166.9000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -708,10 +726,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E151"/>
+  <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D146" sqref="D146"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="D162" sqref="D162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3084,7 +3102,7 @@
         <v>14</v>
       </c>
       <c r="C132">
-        <f t="shared" ref="C132:C151" si="2">(D132-E132)/E132*100</f>
+        <f t="shared" ref="C132:C161" si="2">(D132-E132)/E132*100</f>
         <v>15.838509316770166</v>
       </c>
       <c r="D132">
@@ -3434,6 +3452,186 @@
       </c>
       <c r="E151">
         <v>132.30000000000001</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="A152" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C152">
+        <f t="shared" si="2"/>
+        <v>9.2879256965944279</v>
+      </c>
+      <c r="D152">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="E152">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B153" t="s">
+        <v>5</v>
+      </c>
+      <c r="C153">
+        <f t="shared" si="2"/>
+        <v>-6.666666666666667</v>
+      </c>
+      <c r="D153">
+        <v>7</v>
+      </c>
+      <c r="E153">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
+      <c r="A154" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B154" t="s">
+        <v>6</v>
+      </c>
+      <c r="C154">
+        <f t="shared" si="2"/>
+        <v>19.075144508670526</v>
+      </c>
+      <c r="D154">
+        <v>41.2</v>
+      </c>
+      <c r="E154">
+        <v>34.6</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
+      <c r="A155" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B155" t="s">
+        <v>7</v>
+      </c>
+      <c r="C155">
+        <f t="shared" si="2"/>
+        <v>4.9535603715170327</v>
+      </c>
+      <c r="D155">
+        <v>33.9</v>
+      </c>
+      <c r="E155">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
+      <c r="A156" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B156" t="s">
+        <v>8</v>
+      </c>
+      <c r="C156">
+        <f t="shared" si="2"/>
+        <v>31.150442477876094</v>
+      </c>
+      <c r="D156">
+        <v>296.39999999999998</v>
+      </c>
+      <c r="E156">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
+      <c r="A157" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B157" t="s">
+        <v>9</v>
+      </c>
+      <c r="C157">
+        <f t="shared" si="2"/>
+        <v>52.90102389078497</v>
+      </c>
+      <c r="D157">
+        <v>716.8</v>
+      </c>
+      <c r="E157">
+        <v>468.8</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
+      <c r="A158" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B158" t="s">
+        <v>10</v>
+      </c>
+      <c r="C158">
+        <f t="shared" si="2"/>
+        <v>45.179063360881564</v>
+      </c>
+      <c r="D158">
+        <v>52.7</v>
+      </c>
+      <c r="E158">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
+      <c r="A159" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B159" t="s">
+        <v>11</v>
+      </c>
+      <c r="C159">
+        <f t="shared" si="2"/>
+        <v>15.204678362573084</v>
+      </c>
+      <c r="D159">
+        <v>39.4</v>
+      </c>
+      <c r="E159">
+        <v>34.200000000000003</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
+      <c r="A160" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B160" t="s">
+        <v>12</v>
+      </c>
+      <c r="C160">
+        <f t="shared" si="2"/>
+        <v>33.090024330900249</v>
+      </c>
+      <c r="D160">
+        <v>218.8</v>
+      </c>
+      <c r="E160">
+        <v>164.4</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
+      <c r="A161" s="1">
+        <v>44287</v>
+      </c>
+      <c r="B161" t="s">
+        <v>13</v>
+      </c>
+      <c r="C161">
+        <f t="shared" si="2"/>
+        <v>52.413793103448278</v>
+      </c>
+      <c r="D161">
+        <v>198.9</v>
+      </c>
+      <c r="E161">
+        <v>130.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data: 5 June 2021
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:C17"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C17" si="0">(D3-E3)/E3*100</f>
+        <f t="shared" ref="C3:C18" si="0">(D3-E3)/E3*100</f>
         <v>-2.6758409785932722</v>
       </c>
       <c r="D3">
@@ -716,6 +716,24 @@
       </c>
       <c r="E17">
         <v>1166.9000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>51.088149231894661</v>
+      </c>
+      <c r="D18">
+        <v>1652.3</v>
+      </c>
+      <c r="E18">
+        <v>1093.5999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -726,10 +744,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E161"/>
+  <dimension ref="A1:E171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="D162" sqref="D162"/>
+    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="D172" sqref="D172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3102,7 +3120,7 @@
         <v>14</v>
       </c>
       <c r="C132">
-        <f t="shared" ref="C132:C161" si="2">(D132-E132)/E132*100</f>
+        <f t="shared" ref="C132:C171" si="2">(D132-E132)/E132*100</f>
         <v>15.838509316770166</v>
       </c>
       <c r="D132">
@@ -3632,6 +3650,186 @@
       </c>
       <c r="E161">
         <v>130.5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
+      <c r="A162" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C162">
+        <f t="shared" si="2"/>
+        <v>2.4316109422492533</v>
+      </c>
+      <c r="D162">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="E162">
+        <v>32.9</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
+      <c r="A163" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B163" t="s">
+        <v>5</v>
+      </c>
+      <c r="C163">
+        <f t="shared" si="2"/>
+        <v>10.526315789473696</v>
+      </c>
+      <c r="D163">
+        <v>8.4</v>
+      </c>
+      <c r="E163">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
+      <c r="A164" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B164" t="s">
+        <v>6</v>
+      </c>
+      <c r="C164">
+        <f t="shared" si="2"/>
+        <v>46.666666666666664</v>
+      </c>
+      <c r="D164">
+        <v>48.4</v>
+      </c>
+      <c r="E164">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="A165" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B165" t="s">
+        <v>7</v>
+      </c>
+      <c r="C165">
+        <f t="shared" si="2"/>
+        <v>20.538720538720533</v>
+      </c>
+      <c r="D165">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="E165">
+        <v>29.7</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
+      <c r="A166" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B166" t="s">
+        <v>8</v>
+      </c>
+      <c r="C166">
+        <f t="shared" si="2"/>
+        <v>31.089459698848533</v>
+      </c>
+      <c r="D166">
+        <v>296</v>
+      </c>
+      <c r="E166">
+        <v>225.8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
+      <c r="A167" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B167" t="s">
+        <v>9</v>
+      </c>
+      <c r="C167">
+        <f t="shared" si="2"/>
+        <v>78.432327166504379</v>
+      </c>
+      <c r="D167">
+        <v>733</v>
+      </c>
+      <c r="E167">
+        <v>410.8</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="A168" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B168" t="s">
+        <v>10</v>
+      </c>
+      <c r="C168">
+        <f t="shared" si="2"/>
+        <v>43.502824858757059</v>
+      </c>
+      <c r="D168">
+        <v>50.8</v>
+      </c>
+      <c r="E168">
+        <v>35.4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
+      <c r="A169" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B169" t="s">
+        <v>11</v>
+      </c>
+      <c r="C169">
+        <f t="shared" si="2"/>
+        <v>17.337461300309602</v>
+      </c>
+      <c r="D169">
+        <v>37.9</v>
+      </c>
+      <c r="E169">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
+      <c r="A170" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B170" t="s">
+        <v>12</v>
+      </c>
+      <c r="C170">
+        <f t="shared" si="2"/>
+        <v>28.771289537712885</v>
+      </c>
+      <c r="D170">
+        <v>211.7</v>
+      </c>
+      <c r="E170">
+        <v>164.4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
+      <c r="A171" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B171" t="s">
+        <v>13</v>
+      </c>
+      <c r="C171">
+        <f t="shared" si="2"/>
+        <v>61.626951520131456</v>
+      </c>
+      <c r="D171">
+        <v>196.7</v>
+      </c>
+      <c r="E171">
+        <v>121.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data: 9 July 2021
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C18" si="0">(D3-E3)/E3*100</f>
+        <f t="shared" ref="C3:C19" si="0">(D3-E3)/E3*100</f>
         <v>-2.6758409785932722</v>
       </c>
       <c r="D3">
@@ -734,6 +734,24 @@
       </c>
       <c r="E18">
         <v>1093.5999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>41.224489795918359</v>
+      </c>
+      <c r="D19">
+        <v>1591.6</v>
+      </c>
+      <c r="E19">
+        <v>1127</v>
       </c>
     </row>
   </sheetData>
@@ -744,10 +762,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E171"/>
+  <dimension ref="A1:E181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="D172" sqref="D172"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="D182" sqref="D182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3120,7 +3138,7 @@
         <v>14</v>
       </c>
       <c r="C132">
-        <f t="shared" ref="C132:C171" si="2">(D132-E132)/E132*100</f>
+        <f t="shared" ref="C132:C181" si="2">(D132-E132)/E132*100</f>
         <v>15.838509316770166</v>
       </c>
       <c r="D132">
@@ -3830,6 +3848,186 @@
       </c>
       <c r="E171">
         <v>121.7</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
+      <c r="A172" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C172">
+        <f t="shared" si="2"/>
+        <v>-2.9498525073746311</v>
+      </c>
+      <c r="D172">
+        <v>32.9</v>
+      </c>
+      <c r="E172">
+        <v>33.9</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
+      <c r="A173" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B173" t="s">
+        <v>5</v>
+      </c>
+      <c r="C173">
+        <f t="shared" si="2"/>
+        <v>47.999999999999993</v>
+      </c>
+      <c r="D173">
+        <v>11.1</v>
+      </c>
+      <c r="E173">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
+      <c r="A174" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B174" t="s">
+        <v>6</v>
+      </c>
+      <c r="C174">
+        <f t="shared" si="2"/>
+        <v>31.304347826086946</v>
+      </c>
+      <c r="D174">
+        <v>45.3</v>
+      </c>
+      <c r="E174">
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="A175" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B175" t="s">
+        <v>7</v>
+      </c>
+      <c r="C175">
+        <f t="shared" si="2"/>
+        <v>14.241486068111461</v>
+      </c>
+      <c r="D175">
+        <v>36.9</v>
+      </c>
+      <c r="E175">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
+      <c r="A176" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B176" t="s">
+        <v>8</v>
+      </c>
+      <c r="C176">
+        <f t="shared" si="2"/>
+        <v>28.296826106392498</v>
+      </c>
+      <c r="D176">
+        <v>287</v>
+      </c>
+      <c r="E176">
+        <v>223.7</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B177" t="s">
+        <v>9</v>
+      </c>
+      <c r="C177">
+        <f t="shared" si="2"/>
+        <v>54.421611637035305</v>
+      </c>
+      <c r="D177">
+        <v>668.8</v>
+      </c>
+      <c r="E177">
+        <v>433.1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B178" t="s">
+        <v>10</v>
+      </c>
+      <c r="C178">
+        <f t="shared" si="2"/>
+        <v>36.15384615384616</v>
+      </c>
+      <c r="D178">
+        <v>53.1</v>
+      </c>
+      <c r="E178">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="A179" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B179" t="s">
+        <v>11</v>
+      </c>
+      <c r="C179">
+        <f t="shared" si="2"/>
+        <v>27.936507936507926</v>
+      </c>
+      <c r="D179">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="E179">
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B180" t="s">
+        <v>12</v>
+      </c>
+      <c r="C180">
+        <f t="shared" si="2"/>
+        <v>38.415003024803383</v>
+      </c>
+      <c r="D180">
+        <v>228.8</v>
+      </c>
+      <c r="E180">
+        <v>165.3</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="A181" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B181" t="s">
+        <v>13</v>
+      </c>
+      <c r="C181">
+        <f t="shared" si="2"/>
+        <v>48.415213946117284</v>
+      </c>
+      <c r="D181">
+        <v>187.3</v>
+      </c>
+      <c r="E181">
+        <v>126.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data: 8 August 2021
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C19" si="0">(D3-E3)/E3*100</f>
+        <f t="shared" ref="C3:C20" si="0">(D3-E3)/E3*100</f>
         <v>-2.6758409785932722</v>
       </c>
       <c r="D3">
@@ -752,6 +752,24 @@
       </c>
       <c r="E19">
         <v>1127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>30.558654423753552</v>
+      </c>
+      <c r="D20">
+        <v>1521.4</v>
+      </c>
+      <c r="E20">
+        <v>1165.3</v>
       </c>
     </row>
   </sheetData>
@@ -762,10 +780,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E181"/>
+  <dimension ref="A1:E191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="D182" sqref="D182"/>
+    <sheetView tabSelected="1" topLeftCell="A182" workbookViewId="0">
+      <selection activeCell="D192" sqref="D192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3138,7 +3156,7 @@
         <v>14</v>
       </c>
       <c r="C132">
-        <f t="shared" ref="C132:C181" si="2">(D132-E132)/E132*100</f>
+        <f t="shared" ref="C132:C191" si="2">(D132-E132)/E132*100</f>
         <v>15.838509316770166</v>
       </c>
       <c r="D132">
@@ -4028,6 +4046,186 @@
       </c>
       <c r="E181">
         <v>126.2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
+      <c r="A182" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C182">
+        <f t="shared" si="2"/>
+        <v>-2.4464831804281473</v>
+      </c>
+      <c r="D182">
+        <v>31.9</v>
+      </c>
+      <c r="E182">
+        <v>32.700000000000003</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
+      <c r="A183" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B183" t="s">
+        <v>5</v>
+      </c>
+      <c r="C183">
+        <f t="shared" si="2"/>
+        <v>20.000000000000004</v>
+      </c>
+      <c r="D183">
+        <v>8.4</v>
+      </c>
+      <c r="E183">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
+      <c r="A184" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B184" t="s">
+        <v>6</v>
+      </c>
+      <c r="C184">
+        <f t="shared" si="2"/>
+        <v>12.868632707774811</v>
+      </c>
+      <c r="D184">
+        <v>42.1</v>
+      </c>
+      <c r="E184">
+        <v>37.299999999999997</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="A185" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B185" t="s">
+        <v>7</v>
+      </c>
+      <c r="C185">
+        <f t="shared" si="2"/>
+        <v>7.6246334310850479</v>
+      </c>
+      <c r="D185">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="E185">
+        <v>34.1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
+      <c r="A186" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B186" t="s">
+        <v>8</v>
+      </c>
+      <c r="C186">
+        <f t="shared" si="2"/>
+        <v>22.79314888010542</v>
+      </c>
+      <c r="D186">
+        <v>279.60000000000002</v>
+      </c>
+      <c r="E186">
+        <v>227.7</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5">
+      <c r="A187" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B187" t="s">
+        <v>9</v>
+      </c>
+      <c r="C187">
+        <f t="shared" si="2"/>
+        <v>42.866681504562642</v>
+      </c>
+      <c r="D187">
+        <v>641.9</v>
+      </c>
+      <c r="E187">
+        <v>449.3</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5">
+      <c r="A188" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B188" t="s">
+        <v>10</v>
+      </c>
+      <c r="C188">
+        <f t="shared" si="2"/>
+        <v>6.2656641604010019</v>
+      </c>
+      <c r="D188">
+        <v>42.4</v>
+      </c>
+      <c r="E188">
+        <v>39.9</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
+      <c r="A189" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B189" t="s">
+        <v>11</v>
+      </c>
+      <c r="C189">
+        <f t="shared" si="2"/>
+        <v>23.303834808259584</v>
+      </c>
+      <c r="D189">
+        <v>41.8</v>
+      </c>
+      <c r="E189">
+        <v>33.9</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
+      <c r="A190" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B190" t="s">
+        <v>12</v>
+      </c>
+      <c r="C190">
+        <f t="shared" si="2"/>
+        <v>16.947250280583624</v>
+      </c>
+      <c r="D190">
+        <v>208.4</v>
+      </c>
+      <c r="E190">
+        <v>178.2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5">
+      <c r="A191" s="1">
+        <v>44378</v>
+      </c>
+      <c r="B191" t="s">
+        <v>13</v>
+      </c>
+      <c r="C191">
+        <f t="shared" si="2"/>
+        <v>50.119712689545096</v>
+      </c>
+      <c r="D191">
+        <v>188.1</v>
+      </c>
+      <c r="E191">
+        <v>125.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data: 11 September 2021
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C20" si="0">(D3-E3)/E3*100</f>
+        <f t="shared" ref="C3:C21" si="0">(D3-E3)/E3*100</f>
         <v>-2.6758409785932722</v>
       </c>
       <c r="D3">
@@ -770,6 +770,24 @@
       </c>
       <c r="E20">
         <v>1165.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>22.386537480877113</v>
+      </c>
+      <c r="D21">
+        <v>1440</v>
+      </c>
+      <c r="E21">
+        <v>1176.5999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -780,10 +798,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E191"/>
+  <dimension ref="A1:E201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A182" workbookViewId="0">
-      <selection activeCell="D192" sqref="D192"/>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="D202" sqref="D202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3156,7 +3174,7 @@
         <v>14</v>
       </c>
       <c r="C132">
-        <f t="shared" ref="C132:C191" si="2">(D132-E132)/E132*100</f>
+        <f t="shared" ref="C132:C201" si="2">(D132-E132)/E132*100</f>
         <v>15.838509316770166</v>
       </c>
       <c r="D132">
@@ -4226,6 +4244,186 @@
       </c>
       <c r="E191">
         <v>125.3</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
+      <c r="A192" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C192">
+        <f t="shared" si="2"/>
+        <v>-8.1325301204819365</v>
+      </c>
+      <c r="D192">
+        <v>30.5</v>
+      </c>
+      <c r="E192">
+        <v>33.200000000000003</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
+      <c r="A193" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B193" t="s">
+        <v>5</v>
+      </c>
+      <c r="C193">
+        <f t="shared" si="2"/>
+        <v>25.333333333333336</v>
+      </c>
+      <c r="D193">
+        <v>9.4</v>
+      </c>
+      <c r="E193">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5">
+      <c r="A194" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B194" t="s">
+        <v>6</v>
+      </c>
+      <c r="C194">
+        <f t="shared" si="2"/>
+        <v>-2.2277227722772244</v>
+      </c>
+      <c r="D194">
+        <v>39.5</v>
+      </c>
+      <c r="E194">
+        <v>40.4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5">
+      <c r="A195" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B195" t="s">
+        <v>7</v>
+      </c>
+      <c r="C195">
+        <f t="shared" si="2"/>
+        <v>6.7055393586005954</v>
+      </c>
+      <c r="D195">
+        <v>36.6</v>
+      </c>
+      <c r="E195">
+        <v>34.299999999999997</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5">
+      <c r="A196" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B196" t="s">
+        <v>8</v>
+      </c>
+      <c r="C196">
+        <f t="shared" si="2"/>
+        <v>18.825638727028252</v>
+      </c>
+      <c r="D196">
+        <v>265.10000000000002</v>
+      </c>
+      <c r="E196">
+        <v>223.1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5">
+      <c r="A197" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B197" t="s">
+        <v>9</v>
+      </c>
+      <c r="C197">
+        <f t="shared" si="2"/>
+        <v>36.701170117011706</v>
+      </c>
+      <c r="D197">
+        <v>607.5</v>
+      </c>
+      <c r="E197">
+        <v>444.4</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
+      <c r="A198" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B198" t="s">
+        <v>10</v>
+      </c>
+      <c r="C198">
+        <f t="shared" si="2"/>
+        <v>5.0131926121371997</v>
+      </c>
+      <c r="D198">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="E198">
+        <v>37.9</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5">
+      <c r="A199" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B199" t="s">
+        <v>11</v>
+      </c>
+      <c r="C199">
+        <f t="shared" si="2"/>
+        <v>32.601880877742943</v>
+      </c>
+      <c r="D199">
+        <v>42.3</v>
+      </c>
+      <c r="E199">
+        <v>31.9</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5">
+      <c r="A200" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B200" t="s">
+        <v>12</v>
+      </c>
+      <c r="C200">
+        <f t="shared" si="2"/>
+        <v>6.0307017543859649</v>
+      </c>
+      <c r="D200">
+        <v>193.4</v>
+      </c>
+      <c r="E200">
+        <v>182.4</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5">
+      <c r="A201" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B201" t="s">
+        <v>13</v>
+      </c>
+      <c r="C201">
+        <f t="shared" si="2"/>
+        <v>24.310954063604246</v>
+      </c>
+      <c r="D201">
+        <v>175.9</v>
+      </c>
+      <c r="E201">
+        <v>141.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data: 8 October 2021
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C21" si="0">(D3-E3)/E3*100</f>
+        <f t="shared" ref="C3:C22" si="0">(D3-E3)/E3*100</f>
         <v>-2.6758409785932722</v>
       </c>
       <c r="D3">
@@ -788,6 +788,24 @@
       </c>
       <c r="E21">
         <v>1176.5999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>26.449662041977927</v>
+      </c>
+      <c r="D22">
+        <v>1421.8</v>
+      </c>
+      <c r="E22">
+        <v>1124.4000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -798,10 +816,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E201"/>
+  <dimension ref="A1:E211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="D202" sqref="D202"/>
+    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="D212" sqref="D212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3174,7 +3192,7 @@
         <v>14</v>
       </c>
       <c r="C132">
-        <f t="shared" ref="C132:C201" si="2">(D132-E132)/E132*100</f>
+        <f t="shared" ref="C132:C211" si="2">(D132-E132)/E132*100</f>
         <v>15.838509316770166</v>
       </c>
       <c r="D132">
@@ -4424,6 +4442,186 @@
       </c>
       <c r="E201">
         <v>141.5</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5">
+      <c r="A202" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C202">
+        <f t="shared" si="2"/>
+        <v>12.499999999999984</v>
+      </c>
+      <c r="D202">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="E202">
+        <v>29.6</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5">
+      <c r="A203" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B203" t="s">
+        <v>5</v>
+      </c>
+      <c r="C203">
+        <f t="shared" si="2"/>
+        <v>38.356164383561641</v>
+      </c>
+      <c r="D203">
+        <v>10.1</v>
+      </c>
+      <c r="E203">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5">
+      <c r="A204" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B204" t="s">
+        <v>6</v>
+      </c>
+      <c r="C204">
+        <f t="shared" si="2"/>
+        <v>10.298102981029821</v>
+      </c>
+      <c r="D204">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="E204">
+        <v>36.9</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5">
+      <c r="A205" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B205" t="s">
+        <v>7</v>
+      </c>
+      <c r="C205">
+        <f t="shared" si="2"/>
+        <v>15.217391304347821</v>
+      </c>
+      <c r="D205">
+        <v>37.1</v>
+      </c>
+      <c r="E205">
+        <v>32.200000000000003</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5">
+      <c r="A206" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B206" t="s">
+        <v>8</v>
+      </c>
+      <c r="C206">
+        <f t="shared" si="2"/>
+        <v>13.094209161624883</v>
+      </c>
+      <c r="D206">
+        <v>261.7</v>
+      </c>
+      <c r="E206">
+        <v>231.4</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5">
+      <c r="A207" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B207" t="s">
+        <v>9</v>
+      </c>
+      <c r="C207">
+        <f t="shared" si="2"/>
+        <v>40.924249642686995</v>
+      </c>
+      <c r="D207">
+        <v>591.6</v>
+      </c>
+      <c r="E207">
+        <v>419.8</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
+      <c r="A208" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B208" t="s">
+        <v>10</v>
+      </c>
+      <c r="C208">
+        <f t="shared" si="2"/>
+        <v>16.023738872403555</v>
+      </c>
+      <c r="D208">
+        <v>39.1</v>
+      </c>
+      <c r="E208">
+        <v>33.700000000000003</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5">
+      <c r="A209" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B209" t="s">
+        <v>11</v>
+      </c>
+      <c r="C209">
+        <f t="shared" si="2"/>
+        <v>15.315315315315321</v>
+      </c>
+      <c r="D209">
+        <v>38.4</v>
+      </c>
+      <c r="E209">
+        <v>33.299999999999997</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5">
+      <c r="A210" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B210" t="s">
+        <v>12</v>
+      </c>
+      <c r="C210">
+        <f t="shared" si="2"/>
+        <v>22.384428223844271</v>
+      </c>
+      <c r="D210">
+        <v>201.2</v>
+      </c>
+      <c r="E210">
+        <v>164.4</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5">
+      <c r="A211" s="1">
+        <v>44440</v>
+      </c>
+      <c r="B211" t="s">
+        <v>13</v>
+      </c>
+      <c r="C211">
+        <f t="shared" si="2"/>
+        <v>24.153166421207644</v>
+      </c>
+      <c r="D211">
+        <v>168.6</v>
+      </c>
+      <c r="E211">
+        <v>135.80000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data: 6 November 2021
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C22" si="0">(D3-E3)/E3*100</f>
+        <f t="shared" ref="C3:C23" si="0">(D3-E3)/E3*100</f>
         <v>-2.6758409785932722</v>
       </c>
       <c r="D3">
@@ -806,6 +806,24 @@
       </c>
       <c r="E22">
         <v>1124.4000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1">
+        <v>44470</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>19.957835558678831</v>
+      </c>
+      <c r="D23">
+        <v>1365.6</v>
+      </c>
+      <c r="E23">
+        <v>1138.4000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -816,10 +834,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E211"/>
+  <dimension ref="A1:E221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="D212" sqref="D212"/>
+    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="D222" sqref="D222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3192,7 +3210,7 @@
         <v>14</v>
       </c>
       <c r="C132">
-        <f t="shared" ref="C132:C211" si="2">(D132-E132)/E132*100</f>
+        <f t="shared" ref="C132:C221" si="2">(D132-E132)/E132*100</f>
         <v>15.838509316770166</v>
       </c>
       <c r="D132">
@@ -4622,6 +4640,186 @@
       </c>
       <c r="E211">
         <v>135.80000000000001</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5">
+      <c r="A212" s="1">
+        <v>44470</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C212">
+        <f t="shared" si="2"/>
+        <v>18.394648829431439</v>
+      </c>
+      <c r="D212">
+        <v>35.4</v>
+      </c>
+      <c r="E212">
+        <v>29.9</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5">
+      <c r="A213" s="1">
+        <v>44470</v>
+      </c>
+      <c r="B213" t="s">
+        <v>5</v>
+      </c>
+      <c r="C213">
+        <f t="shared" si="2"/>
+        <v>9.5890410958904138</v>
+      </c>
+      <c r="D213">
+        <v>8</v>
+      </c>
+      <c r="E213">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5">
+      <c r="A214" s="1">
+        <v>44470</v>
+      </c>
+      <c r="B214" t="s">
+        <v>6</v>
+      </c>
+      <c r="C214">
+        <f t="shared" si="2"/>
+        <v>1.6908212560386542</v>
+      </c>
+      <c r="D214">
+        <v>42.1</v>
+      </c>
+      <c r="E214">
+        <v>41.4</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5">
+      <c r="A215" s="1">
+        <v>44470</v>
+      </c>
+      <c r="B215" t="s">
+        <v>7</v>
+      </c>
+      <c r="C215">
+        <f t="shared" si="2"/>
+        <v>14.465408805031441</v>
+      </c>
+      <c r="D215">
+        <v>36.4</v>
+      </c>
+      <c r="E215">
+        <v>31.8</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5">
+      <c r="A216" s="1">
+        <v>44470</v>
+      </c>
+      <c r="B216" t="s">
+        <v>8</v>
+      </c>
+      <c r="C216">
+        <f t="shared" si="2"/>
+        <v>9.1880341880341891</v>
+      </c>
+      <c r="D216">
+        <v>255.5</v>
+      </c>
+      <c r="E216">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5">
+      <c r="A217" s="1">
+        <v>44470</v>
+      </c>
+      <c r="B217" t="s">
+        <v>9</v>
+      </c>
+      <c r="C217">
+        <f t="shared" si="2"/>
+        <v>34.318826868495734</v>
+      </c>
+      <c r="D217">
+        <v>567.9</v>
+      </c>
+      <c r="E217">
+        <v>422.8</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5">
+      <c r="A218" s="1">
+        <v>44470</v>
+      </c>
+      <c r="B218" t="s">
+        <v>10</v>
+      </c>
+      <c r="C218">
+        <f t="shared" si="2"/>
+        <v>1.0899182561307861</v>
+      </c>
+      <c r="D218">
+        <v>37.1</v>
+      </c>
+      <c r="E218">
+        <v>36.700000000000003</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5">
+      <c r="A219" s="1">
+        <v>44470</v>
+      </c>
+      <c r="B219" t="s">
+        <v>11</v>
+      </c>
+      <c r="C219">
+        <f t="shared" si="2"/>
+        <v>15.887850467289724</v>
+      </c>
+      <c r="D219">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="E219">
+        <v>32.1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5">
+      <c r="A220" s="1">
+        <v>44470</v>
+      </c>
+      <c r="B220" t="s">
+        <v>12</v>
+      </c>
+      <c r="C220">
+        <f t="shared" si="2"/>
+        <v>10.523186682520819</v>
+      </c>
+      <c r="D220">
+        <v>185.9</v>
+      </c>
+      <c r="E220">
+        <v>168.2</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5">
+      <c r="A221" s="1">
+        <v>44470</v>
+      </c>
+      <c r="B221" t="s">
+        <v>13</v>
+      </c>
+      <c r="C221">
+        <f t="shared" si="2"/>
+        <v>19.225037257824155</v>
+      </c>
+      <c r="D221">
+        <v>160</v>
+      </c>
+      <c r="E221">
+        <v>134.19999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data: 3 December 2021
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C23" si="0">(D3-E3)/E3*100</f>
+        <f t="shared" ref="C3:C24" si="0">(D3-E3)/E3*100</f>
         <v>-2.6758409785932722</v>
       </c>
       <c r="D3">
@@ -824,6 +824,24 @@
       </c>
       <c r="E23">
         <v>1138.4000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>4.0575587718564377</v>
+      </c>
+      <c r="D24">
+        <v>1243.8</v>
+      </c>
+      <c r="E24">
+        <v>1195.3</v>
       </c>
     </row>
   </sheetData>
@@ -834,10 +852,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E221"/>
+  <dimension ref="A1:E231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
-      <selection activeCell="D222" sqref="D222"/>
+    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
+      <selection activeCell="D232" sqref="D232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3210,7 +3228,7 @@
         <v>14</v>
       </c>
       <c r="C132">
-        <f t="shared" ref="C132:C221" si="2">(D132-E132)/E132*100</f>
+        <f t="shared" ref="C132:C231" si="2">(D132-E132)/E132*100</f>
         <v>15.838509316770166</v>
       </c>
       <c r="D132">
@@ -4820,6 +4838,186 @@
       </c>
       <c r="E221">
         <v>134.19999999999999</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5">
+      <c r="A222" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C222">
+        <f t="shared" si="2"/>
+        <v>-10.738255033557044</v>
+      </c>
+      <c r="D222">
+        <v>26.6</v>
+      </c>
+      <c r="E222">
+        <v>29.8</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5">
+      <c r="A223" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B223" t="s">
+        <v>5</v>
+      </c>
+      <c r="C223">
+        <f t="shared" si="2"/>
+        <v>5.8823529411764763</v>
+      </c>
+      <c r="D223">
+        <v>7.2</v>
+      </c>
+      <c r="E223">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5">
+      <c r="A224" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B224" t="s">
+        <v>6</v>
+      </c>
+      <c r="C224">
+        <f t="shared" si="2"/>
+        <v>3.7406483790523692</v>
+      </c>
+      <c r="D224">
+        <v>41.6</v>
+      </c>
+      <c r="E224">
+        <v>40.1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5">
+      <c r="A225" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B225" t="s">
+        <v>7</v>
+      </c>
+      <c r="C225">
+        <f t="shared" si="2"/>
+        <v>9.6463022508038581</v>
+      </c>
+      <c r="D225">
+        <v>34.1</v>
+      </c>
+      <c r="E225">
+        <v>31.1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5">
+      <c r="A226" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B226" t="s">
+        <v>8</v>
+      </c>
+      <c r="C226">
+        <f t="shared" si="2"/>
+        <v>-19.495864513588028</v>
+      </c>
+      <c r="D226">
+        <v>204.4</v>
+      </c>
+      <c r="E226">
+        <v>253.9</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5">
+      <c r="A227" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B227" t="s">
+        <v>9</v>
+      </c>
+      <c r="C227">
+        <f t="shared" si="2"/>
+        <v>19.498158379373862</v>
+      </c>
+      <c r="D227">
+        <v>519.1</v>
+      </c>
+      <c r="E227">
+        <v>434.4</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5">
+      <c r="A228" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B228" t="s">
+        <v>10</v>
+      </c>
+      <c r="C228">
+        <f t="shared" si="2"/>
+        <v>-8.9974293059125969</v>
+      </c>
+      <c r="D228">
+        <v>35.4</v>
+      </c>
+      <c r="E228">
+        <v>38.9</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5">
+      <c r="A229" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B229" t="s">
+        <v>11</v>
+      </c>
+      <c r="C229">
+        <f t="shared" si="2"/>
+        <v>-16.393442622950818</v>
+      </c>
+      <c r="D229">
+        <v>30.6</v>
+      </c>
+      <c r="E229">
+        <v>36.6</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5">
+      <c r="A230" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B230" t="s">
+        <v>12</v>
+      </c>
+      <c r="C230">
+        <f t="shared" si="2"/>
+        <v>2.1393307734503439</v>
+      </c>
+      <c r="D230">
+        <v>186.2</v>
+      </c>
+      <c r="E230">
+        <v>182.3</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5">
+      <c r="A231" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B231" t="s">
+        <v>13</v>
+      </c>
+      <c r="C231">
+        <f t="shared" si="2"/>
+        <v>12.25212464589236</v>
+      </c>
+      <c r="D231">
+        <v>158.5</v>
+      </c>
+      <c r="E231">
+        <v>141.19999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upload data: 15 January 2022
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C24" si="0">(D3-E3)/E3*100</f>
+        <f t="shared" ref="C3:C25" si="0">(D3-E3)/E3*100</f>
         <v>-2.6758409785932722</v>
       </c>
       <c r="D3">
@@ -842,6 +842,24 @@
       </c>
       <c r="E24">
         <v>1195.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>5.5366936536954734</v>
+      </c>
+      <c r="D25">
+        <v>1212.3</v>
+      </c>
+      <c r="E25">
+        <v>1148.7</v>
       </c>
     </row>
   </sheetData>
@@ -852,10 +870,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E231"/>
+  <dimension ref="A1:E241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
-      <selection activeCell="D232" sqref="D232"/>
+    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
+      <selection activeCell="D242" sqref="D242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3228,7 +3246,7 @@
         <v>14</v>
       </c>
       <c r="C132">
-        <f t="shared" ref="C132:C231" si="2">(D132-E132)/E132*100</f>
+        <f t="shared" ref="C132:C241" si="2">(D132-E132)/E132*100</f>
         <v>15.838509316770166</v>
       </c>
       <c r="D132">
@@ -5018,6 +5036,186 @@
       </c>
       <c r="E231">
         <v>141.19999999999999</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5">
+      <c r="A232" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C232">
+        <f t="shared" si="2"/>
+        <v>-6.0509554140127344</v>
+      </c>
+      <c r="D232">
+        <v>29.5</v>
+      </c>
+      <c r="E232">
+        <v>31.4</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5">
+      <c r="A233" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B233" t="s">
+        <v>5</v>
+      </c>
+      <c r="C233">
+        <f t="shared" si="2"/>
+        <v>2.9411764705882382</v>
+      </c>
+      <c r="D233">
+        <v>7</v>
+      </c>
+      <c r="E233">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5">
+      <c r="A234" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B234" t="s">
+        <v>6</v>
+      </c>
+      <c r="C234">
+        <f t="shared" si="2"/>
+        <v>-0.49627791563274376</v>
+      </c>
+      <c r="D234">
+        <v>40.1</v>
+      </c>
+      <c r="E234">
+        <v>40.299999999999997</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5">
+      <c r="A235" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B235" t="s">
+        <v>7</v>
+      </c>
+      <c r="C235">
+        <f t="shared" si="2"/>
+        <v>5.7239057239057214</v>
+      </c>
+      <c r="D235">
+        <v>31.4</v>
+      </c>
+      <c r="E235">
+        <v>29.7</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5">
+      <c r="A236" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B236" t="s">
+        <v>8</v>
+      </c>
+      <c r="C236">
+        <f t="shared" si="2"/>
+        <v>-10.85762568652302</v>
+      </c>
+      <c r="D236">
+        <v>211</v>
+      </c>
+      <c r="E236">
+        <v>236.7</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5">
+      <c r="A237" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B237" t="s">
+        <v>9</v>
+      </c>
+      <c r="C237">
+        <f t="shared" si="2"/>
+        <v>17.202763878961161</v>
+      </c>
+      <c r="D237">
+        <v>491.9</v>
+      </c>
+      <c r="E237">
+        <v>419.7</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5">
+      <c r="A238" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B238" t="s">
+        <v>10</v>
+      </c>
+      <c r="C238">
+        <f t="shared" si="2"/>
+        <v>3.7037037037036953</v>
+      </c>
+      <c r="D238">
+        <v>36.4</v>
+      </c>
+      <c r="E238">
+        <v>35.1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5">
+      <c r="A239" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B239" t="s">
+        <v>11</v>
+      </c>
+      <c r="C239">
+        <f t="shared" si="2"/>
+        <v>-10.192837465564727</v>
+      </c>
+      <c r="D239">
+        <v>32.6</v>
+      </c>
+      <c r="E239">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5">
+      <c r="A240" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B240" t="s">
+        <v>12</v>
+      </c>
+      <c r="C240">
+        <f t="shared" si="2"/>
+        <v>1.6246498599439809</v>
+      </c>
+      <c r="D240">
+        <v>181.4</v>
+      </c>
+      <c r="E240">
+        <v>178.5</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5">
+      <c r="A241" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B241" t="s">
+        <v>13</v>
+      </c>
+      <c r="C241">
+        <f t="shared" si="2"/>
+        <v>12.602535421327371</v>
+      </c>
+      <c r="D241">
+        <v>151</v>
+      </c>
+      <c r="E241">
+        <v>134.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data: 4 February 2022
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C25" si="0">(D3-E3)/E3*100</f>
+        <f t="shared" ref="C3:C26" si="0">(D3-E3)/E3*100</f>
         <v>-2.6758409785932722</v>
       </c>
       <c r="D3">
@@ -860,6 +860,24 @@
       </c>
       <c r="E25">
         <v>1148.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1">
+        <v>44562</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>13.625201117791502</v>
+      </c>
+      <c r="D26">
+        <v>1341.8</v>
+      </c>
+      <c r="E26">
+        <v>1180.9000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -870,10 +888,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E241"/>
+  <dimension ref="A1:E251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
-      <selection activeCell="D242" sqref="D242"/>
+    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
+      <selection activeCell="D252" sqref="D252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3246,7 +3264,7 @@
         <v>14</v>
       </c>
       <c r="C132">
-        <f t="shared" ref="C132:C241" si="2">(D132-E132)/E132*100</f>
+        <f t="shared" ref="C132:C251" si="2">(D132-E132)/E132*100</f>
         <v>15.838509316770166</v>
       </c>
       <c r="D132">
@@ -5215,6 +5233,186 @@
         <v>151</v>
       </c>
       <c r="E241">
+        <v>134.1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5">
+      <c r="A242" s="1">
+        <v>44562</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C242">
+        <f t="shared" si="2"/>
+        <v>2.8753993610223709</v>
+      </c>
+      <c r="D242">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="E242">
+        <v>31.3</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5">
+      <c r="A243" s="1">
+        <v>44562</v>
+      </c>
+      <c r="B243" t="s">
+        <v>5</v>
+      </c>
+      <c r="C243">
+        <f t="shared" si="2"/>
+        <v>4.8780487804878101</v>
+      </c>
+      <c r="D243">
+        <v>8.6</v>
+      </c>
+      <c r="E243">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5">
+      <c r="A244" s="1">
+        <v>44562</v>
+      </c>
+      <c r="B244" t="s">
+        <v>6</v>
+      </c>
+      <c r="C244">
+        <f t="shared" si="2"/>
+        <v>1.9943019943019822</v>
+      </c>
+      <c r="D244">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="E244">
+        <v>35.1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5">
+      <c r="A245" s="1">
+        <v>44562</v>
+      </c>
+      <c r="B245" t="s">
+        <v>7</v>
+      </c>
+      <c r="C245">
+        <f t="shared" si="2"/>
+        <v>3.4055727554179613</v>
+      </c>
+      <c r="D245">
+        <v>33.4</v>
+      </c>
+      <c r="E245">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5">
+      <c r="A246" s="1">
+        <v>44562</v>
+      </c>
+      <c r="B246" t="s">
+        <v>8</v>
+      </c>
+      <c r="C246">
+        <f t="shared" si="2"/>
+        <v>2.1056977704376645</v>
+      </c>
+      <c r="D246">
+        <v>247.3</v>
+      </c>
+      <c r="E246">
+        <v>242.2</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5">
+      <c r="A247" s="1">
+        <v>44562</v>
+      </c>
+      <c r="B247" t="s">
+        <v>9</v>
+      </c>
+      <c r="C247">
+        <f t="shared" si="2"/>
+        <v>29.579316389132345</v>
+      </c>
+      <c r="D247">
+        <v>591.4</v>
+      </c>
+      <c r="E247">
+        <v>456.4</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5">
+      <c r="A248" s="1">
+        <v>44562</v>
+      </c>
+      <c r="B248" t="s">
+        <v>10</v>
+      </c>
+      <c r="C248">
+        <f t="shared" si="2"/>
+        <v>-11.691542288557221</v>
+      </c>
+      <c r="D248">
+        <v>35.5</v>
+      </c>
+      <c r="E248">
+        <v>40.200000000000003</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5">
+      <c r="A249" s="1">
+        <v>44562</v>
+      </c>
+      <c r="B249" t="s">
+        <v>11</v>
+      </c>
+      <c r="C249">
+        <f t="shared" si="2"/>
+        <v>-2.3460410557184876</v>
+      </c>
+      <c r="D249">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="E249">
+        <v>34.1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5">
+      <c r="A250" s="1">
+        <v>44562</v>
+      </c>
+      <c r="B250" t="s">
+        <v>12</v>
+      </c>
+      <c r="C250">
+        <f t="shared" si="2"/>
+        <v>7.7245508982035958</v>
+      </c>
+      <c r="D250">
+        <v>179.9</v>
+      </c>
+      <c r="E250">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5">
+      <c r="A251" s="1">
+        <v>44562</v>
+      </c>
+      <c r="B251" t="s">
+        <v>13</v>
+      </c>
+      <c r="C251">
+        <f t="shared" si="2"/>
+        <v>7.6062639821029219</v>
+      </c>
+      <c r="D251">
+        <v>144.30000000000001</v>
+      </c>
+      <c r="E251">
         <v>134.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update data: 11 March 2022
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C26" si="0">(D3-E3)/E3*100</f>
+        <f t="shared" ref="C3:C27" si="0">(D3-E3)/E3*100</f>
         <v>-2.6758409785932722</v>
       </c>
       <c r="D3">
@@ -878,6 +878,24 @@
       </c>
       <c r="E26">
         <v>1180.9000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>-3.5423037716615737</v>
+      </c>
+      <c r="D27">
+        <v>1135.5</v>
+      </c>
+      <c r="E27">
+        <v>1177.2</v>
       </c>
     </row>
   </sheetData>
@@ -888,10 +906,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E251"/>
+  <dimension ref="A1:E261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="D252" sqref="D252"/>
+    <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
+      <selection activeCell="D262" sqref="D262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3264,7 +3282,7 @@
         <v>14</v>
       </c>
       <c r="C132">
-        <f t="shared" ref="C132:C251" si="2">(D132-E132)/E132*100</f>
+        <f t="shared" ref="C132:C261" si="2">(D132-E132)/E132*100</f>
         <v>15.838509316770166</v>
       </c>
       <c r="D132">
@@ -5414,6 +5432,186 @@
       </c>
       <c r="E251">
         <v>134.1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5">
+      <c r="A252" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C252">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D252">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="E252">
+        <v>32.200000000000003</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5">
+      <c r="A253" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B253" t="s">
+        <v>5</v>
+      </c>
+      <c r="C253">
+        <f t="shared" si="2"/>
+        <v>-2.3529411764705799</v>
+      </c>
+      <c r="D253">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E253">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5">
+      <c r="A254" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B254" t="s">
+        <v>6</v>
+      </c>
+      <c r="C254">
+        <f t="shared" si="2"/>
+        <v>2.127659574468094</v>
+      </c>
+      <c r="D254">
+        <v>33.6</v>
+      </c>
+      <c r="E254">
+        <v>32.9</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5">
+      <c r="A255" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B255" t="s">
+        <v>7</v>
+      </c>
+      <c r="C255">
+        <f t="shared" si="2"/>
+        <v>-9.5930232558139448</v>
+      </c>
+      <c r="D255">
+        <v>31.1</v>
+      </c>
+      <c r="E255">
+        <v>34.4</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5">
+      <c r="A256" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B256" t="s">
+        <v>8</v>
+      </c>
+      <c r="C256">
+        <f t="shared" si="2"/>
+        <v>-15.77235772357724</v>
+      </c>
+      <c r="D256">
+        <v>207.2</v>
+      </c>
+      <c r="E256">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5">
+      <c r="A257" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B257" t="s">
+        <v>9</v>
+      </c>
+      <c r="C257">
+        <f t="shared" si="2"/>
+        <v>1.2561686855091891</v>
+      </c>
+      <c r="D257">
+        <v>451.4</v>
+      </c>
+      <c r="E257">
+        <v>445.8</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5">
+      <c r="A258" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B258" t="s">
+        <v>10</v>
+      </c>
+      <c r="C258">
+        <f t="shared" si="2"/>
+        <v>-8.3333333333333375</v>
+      </c>
+      <c r="D258">
+        <v>34.1</v>
+      </c>
+      <c r="E258">
+        <v>37.200000000000003</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5">
+      <c r="A259" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B259" t="s">
+        <v>11</v>
+      </c>
+      <c r="C259">
+        <f t="shared" si="2"/>
+        <v>-18.233618233618241</v>
+      </c>
+      <c r="D259">
+        <v>28.7</v>
+      </c>
+      <c r="E259">
+        <v>35.1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5">
+      <c r="A260" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B260" t="s">
+        <v>12</v>
+      </c>
+      <c r="C260">
+        <f t="shared" si="2"/>
+        <v>-5.4809843400447482</v>
+      </c>
+      <c r="D260">
+        <v>169</v>
+      </c>
+      <c r="E260">
+        <v>178.8</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5">
+      <c r="A261" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B261" t="s">
+        <v>13</v>
+      </c>
+      <c r="C261">
+        <f t="shared" si="2"/>
+        <v>10.935023771790805</v>
+      </c>
+      <c r="D261">
+        <v>140</v>
+      </c>
+      <c r="E261">
+        <v>126.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data: 8 April 2022
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C27" si="0">(D3-E3)/E3*100</f>
+        <f t="shared" ref="C3:C28" si="0">(D3-E3)/E3*100</f>
         <v>-2.6758409785932722</v>
       </c>
       <c r="D3">
@@ -896,6 +896,24 @@
       </c>
       <c r="E27">
         <v>1177.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>-5.9014710913445088</v>
+      </c>
+      <c r="D28">
+        <v>1100.2</v>
+      </c>
+      <c r="E28">
+        <v>1169.2</v>
       </c>
     </row>
   </sheetData>
@@ -906,10 +924,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E261"/>
+  <dimension ref="A1:E271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
-      <selection activeCell="D262" sqref="D262"/>
+    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
+      <selection activeCell="D272" sqref="D272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3282,7 +3300,7 @@
         <v>14</v>
       </c>
       <c r="C132">
-        <f t="shared" ref="C132:C261" si="2">(D132-E132)/E132*100</f>
+        <f t="shared" ref="C132:C271" si="2">(D132-E132)/E132*100</f>
         <v>15.838509316770166</v>
       </c>
       <c r="D132">
@@ -5612,6 +5630,186 @@
       </c>
       <c r="E261">
         <v>126.2</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5">
+      <c r="A262" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C262">
+        <f t="shared" si="2"/>
+        <v>5.379746835443024</v>
+      </c>
+      <c r="D262">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="E262">
+        <v>31.6</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5">
+      <c r="A263" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B263" t="s">
+        <v>5</v>
+      </c>
+      <c r="C263">
+        <f t="shared" si="2"/>
+        <v>-1.315789473684206</v>
+      </c>
+      <c r="D263">
+        <v>7.5</v>
+      </c>
+      <c r="E263">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5">
+      <c r="A264" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B264" t="s">
+        <v>6</v>
+      </c>
+      <c r="C264">
+        <f t="shared" si="2"/>
+        <v>2.4999999999999911</v>
+      </c>
+      <c r="D264">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="E264">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5">
+      <c r="A265" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B265" t="s">
+        <v>7</v>
+      </c>
+      <c r="C265">
+        <f t="shared" si="2"/>
+        <v>-3.7974683544303889</v>
+      </c>
+      <c r="D265">
+        <v>30.4</v>
+      </c>
+      <c r="E265">
+        <v>31.6</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5">
+      <c r="A266" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B266" t="s">
+        <v>8</v>
+      </c>
+      <c r="C266">
+        <f t="shared" si="2"/>
+        <v>-20.335429769392032</v>
+      </c>
+      <c r="D266">
+        <v>190</v>
+      </c>
+      <c r="E266">
+        <v>238.5</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5">
+      <c r="A267" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B267" t="s">
+        <v>9</v>
+      </c>
+      <c r="C267">
+        <f t="shared" si="2"/>
+        <v>-7.0501730103806155</v>
+      </c>
+      <c r="D267">
+        <v>429.8</v>
+      </c>
+      <c r="E267">
+        <v>462.4</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5">
+      <c r="A268" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B268" t="s">
+        <v>10</v>
+      </c>
+      <c r="C268">
+        <f t="shared" si="2"/>
+        <v>3.3519553072625783</v>
+      </c>
+      <c r="D268">
+        <v>37</v>
+      </c>
+      <c r="E268">
+        <v>35.799999999999997</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5">
+      <c r="A269" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B269" t="s">
+        <v>11</v>
+      </c>
+      <c r="C269">
+        <f t="shared" si="2"/>
+        <v>-0.3267973856209197</v>
+      </c>
+      <c r="D269">
+        <v>30.5</v>
+      </c>
+      <c r="E269">
+        <v>30.6</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5">
+      <c r="A270" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B270" t="s">
+        <v>12</v>
+      </c>
+      <c r="C270">
+        <f t="shared" si="2"/>
+        <v>-2.6363091671659711</v>
+      </c>
+      <c r="D270">
+        <v>162.5</v>
+      </c>
+      <c r="E270">
+        <v>166.9</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5">
+      <c r="A271" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B271" t="s">
+        <v>13</v>
+      </c>
+      <c r="C271">
+        <f t="shared" si="2"/>
+        <v>10.657596371882081</v>
+      </c>
+      <c r="D271">
+        <v>146.4</v>
+      </c>
+      <c r="E271">
+        <v>132.30000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New data: 9 May 2022
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C28" si="0">(D3-E3)/E3*100</f>
+        <f t="shared" ref="C3:C29" si="0">(D3-E3)/E3*100</f>
         <v>-2.6758409785932722</v>
       </c>
       <c r="D3">
@@ -914,6 +914,24 @@
       </c>
       <c r="E28">
         <v>1169.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1">
+        <v>44652</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>-6.9500385637158395</v>
+      </c>
+      <c r="D29">
+        <v>1085.8</v>
+      </c>
+      <c r="E29">
+        <v>1166.9000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -924,10 +942,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E271"/>
+  <dimension ref="A1:E281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
-      <selection activeCell="D272" sqref="D272"/>
+    <sheetView tabSelected="1" topLeftCell="A267" workbookViewId="0">
+      <selection activeCell="D282" sqref="D282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3300,7 +3318,7 @@
         <v>14</v>
       </c>
       <c r="C132">
-        <f t="shared" ref="C132:C271" si="2">(D132-E132)/E132*100</f>
+        <f t="shared" ref="C132:C281" si="2">(D132-E132)/E132*100</f>
         <v>15.838509316770166</v>
       </c>
       <c r="D132">
@@ -5810,6 +5828,186 @@
       </c>
       <c r="E271">
         <v>132.30000000000001</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5">
+      <c r="A272" s="1">
+        <v>44652</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C272">
+        <f t="shared" si="2"/>
+        <v>-14.551083591331256</v>
+      </c>
+      <c r="D272">
+        <v>27.6</v>
+      </c>
+      <c r="E272">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5">
+      <c r="A273" s="1">
+        <v>44652</v>
+      </c>
+      <c r="B273" t="s">
+        <v>5</v>
+      </c>
+      <c r="C273">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D273">
+        <v>7.5</v>
+      </c>
+      <c r="E273">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5">
+      <c r="A274" s="1">
+        <v>44652</v>
+      </c>
+      <c r="B274" t="s">
+        <v>6</v>
+      </c>
+      <c r="C274">
+        <f t="shared" si="2"/>
+        <v>-11.560693641618498</v>
+      </c>
+      <c r="D274">
+        <v>30.6</v>
+      </c>
+      <c r="E274">
+        <v>34.6</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5">
+      <c r="A275" s="1">
+        <v>44652</v>
+      </c>
+      <c r="B275" t="s">
+        <v>7</v>
+      </c>
+      <c r="C275">
+        <f t="shared" si="2"/>
+        <v>-13.312693498452004</v>
+      </c>
+      <c r="D275">
+        <v>28</v>
+      </c>
+      <c r="E275">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5">
+      <c r="A276" s="1">
+        <v>44652</v>
+      </c>
+      <c r="B276" t="s">
+        <v>8</v>
+      </c>
+      <c r="C276">
+        <f t="shared" si="2"/>
+        <v>-20.530973451327437</v>
+      </c>
+      <c r="D276">
+        <v>179.6</v>
+      </c>
+      <c r="E276">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5">
+      <c r="A277" s="1">
+        <v>44652</v>
+      </c>
+      <c r="B277" t="s">
+        <v>9</v>
+      </c>
+      <c r="C277">
+        <f t="shared" si="2"/>
+        <v>-5.8020477815699634</v>
+      </c>
+      <c r="D277">
+        <v>441.6</v>
+      </c>
+      <c r="E277">
+        <v>468.8</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5">
+      <c r="A278" s="1">
+        <v>44652</v>
+      </c>
+      <c r="B278" t="s">
+        <v>10</v>
+      </c>
+      <c r="C278">
+        <f t="shared" si="2"/>
+        <v>-3.0303030303030147</v>
+      </c>
+      <c r="D278">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="E278">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5">
+      <c r="A279" s="1">
+        <v>44652</v>
+      </c>
+      <c r="B279" t="s">
+        <v>11</v>
+      </c>
+      <c r="C279">
+        <f t="shared" si="2"/>
+        <v>-2.6315789473684377</v>
+      </c>
+      <c r="D279">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="E279">
+        <v>34.200000000000003</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5">
+      <c r="A280" s="1">
+        <v>44652</v>
+      </c>
+      <c r="B280" t="s">
+        <v>12</v>
+      </c>
+      <c r="C280">
+        <f t="shared" si="2"/>
+        <v>-10.705596107055957</v>
+      </c>
+      <c r="D280">
+        <v>146.80000000000001</v>
+      </c>
+      <c r="E280">
+        <v>164.4</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5">
+      <c r="A281" s="1">
+        <v>44652</v>
+      </c>
+      <c r="B281" t="s">
+        <v>13</v>
+      </c>
+      <c r="C281">
+        <f t="shared" si="2"/>
+        <v>19.233716475095779</v>
+      </c>
+      <c r="D281">
+        <v>155.6</v>
+      </c>
+      <c r="E281">
+        <v>130.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data: 10 June 2022
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C29" si="0">(D3-E3)/E3*100</f>
+        <f t="shared" ref="C3:C30" si="0">(D3-E3)/E3*100</f>
         <v>-2.6758409785932722</v>
       </c>
       <c r="D3">
@@ -932,6 +932,24 @@
       </c>
       <c r="E29">
         <v>1166.9000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>-3.2735918068763676</v>
+      </c>
+      <c r="D30">
+        <v>1057.8</v>
+      </c>
+      <c r="E30">
+        <v>1093.5999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -942,10 +960,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E281"/>
+  <dimension ref="A1:E291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A267" workbookViewId="0">
-      <selection activeCell="D282" sqref="D282"/>
+    <sheetView tabSelected="1" topLeftCell="A275" workbookViewId="0">
+      <selection activeCell="D292" sqref="D292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3318,7 +3336,7 @@
         <v>14</v>
       </c>
       <c r="C132">
-        <f t="shared" ref="C132:C281" si="2">(D132-E132)/E132*100</f>
+        <f t="shared" ref="C132:C291" si="2">(D132-E132)/E132*100</f>
         <v>15.838509316770166</v>
       </c>
       <c r="D132">
@@ -6008,6 +6026,186 @@
       </c>
       <c r="E281">
         <v>130.5</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5">
+      <c r="A282" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C282">
+        <f t="shared" si="2"/>
+        <v>-21.88449848024316</v>
+      </c>
+      <c r="D282">
+        <v>25.7</v>
+      </c>
+      <c r="E282">
+        <v>32.9</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5">
+      <c r="A283" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B283" t="s">
+        <v>5</v>
+      </c>
+      <c r="C283">
+        <f t="shared" si="2"/>
+        <v>-5.2631578947368354</v>
+      </c>
+      <c r="D283">
+        <v>7.2</v>
+      </c>
+      <c r="E283">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5">
+      <c r="A284" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B284" t="s">
+        <v>6</v>
+      </c>
+      <c r="C284">
+        <f t="shared" si="2"/>
+        <v>3.9393939393939306</v>
+      </c>
+      <c r="D284">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="E284">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5">
+      <c r="A285" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B285" t="s">
+        <v>7</v>
+      </c>
+      <c r="C285">
+        <f t="shared" si="2"/>
+        <v>-6.0606060606060632</v>
+      </c>
+      <c r="D285">
+        <v>27.9</v>
+      </c>
+      <c r="E285">
+        <v>29.7</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5">
+      <c r="A286" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B286" t="s">
+        <v>8</v>
+      </c>
+      <c r="C286">
+        <f t="shared" si="2"/>
+        <v>-14.570416297608505</v>
+      </c>
+      <c r="D286">
+        <v>192.9</v>
+      </c>
+      <c r="E286">
+        <v>225.8</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5">
+      <c r="A287" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B287" t="s">
+        <v>9</v>
+      </c>
+      <c r="C287">
+        <f t="shared" si="2"/>
+        <v>8.9824732229795465</v>
+      </c>
+      <c r="D287">
+        <v>447.7</v>
+      </c>
+      <c r="E287">
+        <v>410.8</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5">
+      <c r="A288" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B288" t="s">
+        <v>10</v>
+      </c>
+      <c r="C288">
+        <f t="shared" si="2"/>
+        <v>-7.3446327683615866</v>
+      </c>
+      <c r="D288">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="E288">
+        <v>35.4</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5">
+      <c r="A289" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B289" t="s">
+        <v>11</v>
+      </c>
+      <c r="C289">
+        <f t="shared" si="2"/>
+        <v>-10.216718266253862</v>
+      </c>
+      <c r="D289">
+        <v>29</v>
+      </c>
+      <c r="E289">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5">
+      <c r="A290" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B290" t="s">
+        <v>12</v>
+      </c>
+      <c r="C290">
+        <f t="shared" si="2"/>
+        <v>-19.951338199513387</v>
+      </c>
+      <c r="D290">
+        <v>131.6</v>
+      </c>
+      <c r="E290">
+        <v>164.4</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5">
+      <c r="A291" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B291" t="s">
+        <v>13</v>
+      </c>
+      <c r="C291">
+        <f t="shared" si="2"/>
+        <v>5.6696795398520887</v>
+      </c>
+      <c r="D291">
+        <v>128.6</v>
+      </c>
+      <c r="E291">
+        <v>121.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data: 18 July 2022
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C30" si="0">(D3-E3)/E3*100</f>
+        <f t="shared" ref="C3:C31" si="0">(D3-E3)/E3*100</f>
         <v>-2.6758409785932722</v>
       </c>
       <c r="D3">
@@ -950,6 +950,24 @@
       </c>
       <c r="E30">
         <v>1093.5999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>-10.95829636202307</v>
+      </c>
+      <c r="D31">
+        <v>1003.5</v>
+      </c>
+      <c r="E31">
+        <v>1127</v>
       </c>
     </row>
   </sheetData>
@@ -960,10 +978,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E291"/>
+  <dimension ref="A1:E301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A275" workbookViewId="0">
-      <selection activeCell="D292" sqref="D292"/>
+    <sheetView tabSelected="1" topLeftCell="A285" workbookViewId="0">
+      <selection activeCell="D302" sqref="D302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3336,7 +3354,7 @@
         <v>14</v>
       </c>
       <c r="C132">
-        <f t="shared" ref="C132:C291" si="2">(D132-E132)/E132*100</f>
+        <f t="shared" ref="C132:C301" si="2">(D132-E132)/E132*100</f>
         <v>15.838509316770166</v>
       </c>
       <c r="D132">
@@ -6206,6 +6224,186 @@
       </c>
       <c r="E291">
         <v>121.7</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5">
+      <c r="A292" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C292">
+        <f t="shared" si="2"/>
+        <v>-25.663716814159294</v>
+      </c>
+      <c r="D292">
+        <v>25.2</v>
+      </c>
+      <c r="E292">
+        <v>33.9</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5">
+      <c r="A293" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B293" t="s">
+        <v>5</v>
+      </c>
+      <c r="C293">
+        <f t="shared" si="2"/>
+        <v>-40</v>
+      </c>
+      <c r="D293">
+        <v>4.5</v>
+      </c>
+      <c r="E293">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5">
+      <c r="A294" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B294" t="s">
+        <v>6</v>
+      </c>
+      <c r="C294">
+        <f t="shared" si="2"/>
+        <v>4.0579710144927494</v>
+      </c>
+      <c r="D294">
+        <v>35.9</v>
+      </c>
+      <c r="E294">
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5">
+      <c r="A295" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B295" t="s">
+        <v>7</v>
+      </c>
+      <c r="C295">
+        <f t="shared" si="2"/>
+        <v>-25.696594427244573</v>
+      </c>
+      <c r="D295">
+        <v>24</v>
+      </c>
+      <c r="E295">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5">
+      <c r="A296" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B296" t="s">
+        <v>8</v>
+      </c>
+      <c r="C296">
+        <f t="shared" si="2"/>
+        <v>-13.32141260616897</v>
+      </c>
+      <c r="D296">
+        <v>193.9</v>
+      </c>
+      <c r="E296">
+        <v>223.7</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5">
+      <c r="A297" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B297" t="s">
+        <v>9</v>
+      </c>
+      <c r="C297">
+        <f t="shared" si="2"/>
+        <v>-4.1560840452551373</v>
+      </c>
+      <c r="D297">
+        <v>415.1</v>
+      </c>
+      <c r="E297">
+        <v>433.1</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5">
+      <c r="A298" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B298" t="s">
+        <v>10</v>
+      </c>
+      <c r="C298">
+        <f t="shared" si="2"/>
+        <v>-32.051282051282051</v>
+      </c>
+      <c r="D298">
+        <v>26.5</v>
+      </c>
+      <c r="E298">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5">
+      <c r="A299" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B299" t="s">
+        <v>11</v>
+      </c>
+      <c r="C299">
+        <f t="shared" si="2"/>
+        <v>-25.079365079365072</v>
+      </c>
+      <c r="D299">
+        <v>23.6</v>
+      </c>
+      <c r="E299">
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5">
+      <c r="A300" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B300" t="s">
+        <v>12</v>
+      </c>
+      <c r="C300">
+        <f t="shared" si="2"/>
+        <v>-25.892316999395042</v>
+      </c>
+      <c r="D300">
+        <v>122.5</v>
+      </c>
+      <c r="E300">
+        <v>165.3</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5">
+      <c r="A301" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B301" t="s">
+        <v>13</v>
+      </c>
+      <c r="C301">
+        <f t="shared" si="2"/>
+        <v>4.7543581616481658</v>
+      </c>
+      <c r="D301">
+        <v>132.19999999999999</v>
+      </c>
+      <c r="E301">
+        <v>126.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data: 5 August 2022
</commit_message>
<xml_diff>
--- a/input_data/Unemployment.xlsx
+++ b/input_data/Unemployment.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -456,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C31" si="0">(D3-E3)/E3*100</f>
+        <f t="shared" ref="C3:C32" si="0">(D3-E3)/E3*100</f>
         <v>-2.6758409785932722</v>
       </c>
       <c r="D3">
@@ -968,6 +968,24 @@
       </c>
       <c r="E31">
         <v>1127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>-13.575903200892469</v>
+      </c>
+      <c r="D32">
+        <v>1007.1</v>
+      </c>
+      <c r="E32">
+        <v>1165.3</v>
       </c>
     </row>
   </sheetData>
@@ -978,10 +996,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E301"/>
+  <dimension ref="A1:E311"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A285" workbookViewId="0">
-      <selection activeCell="D302" sqref="D302"/>
+    <sheetView tabSelected="1" topLeftCell="A297" workbookViewId="0">
+      <selection activeCell="D312" sqref="D312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3354,7 +3372,7 @@
         <v>14</v>
       </c>
       <c r="C132">
-        <f t="shared" ref="C132:C301" si="2">(D132-E132)/E132*100</f>
+        <f t="shared" ref="C132:C311" si="2">(D132-E132)/E132*100</f>
         <v>15.838509316770166</v>
       </c>
       <c r="D132">
@@ -6404,6 +6422,186 @@
       </c>
       <c r="E301">
         <v>126.2</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5">
+      <c r="A302" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B302" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C302">
+        <f t="shared" si="2"/>
+        <v>-21.100917431192663</v>
+      </c>
+      <c r="D302">
+        <v>25.8</v>
+      </c>
+      <c r="E302">
+        <v>32.700000000000003</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5">
+      <c r="A303" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B303" t="s">
+        <v>5</v>
+      </c>
+      <c r="C303">
+        <f t="shared" si="2"/>
+        <v>-27.142857142857146</v>
+      </c>
+      <c r="D303">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E303">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5">
+      <c r="A304" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B304" t="s">
+        <v>6</v>
+      </c>
+      <c r="C304">
+        <f t="shared" si="2"/>
+        <v>-19.571045576407499</v>
+      </c>
+      <c r="D304">
+        <v>30</v>
+      </c>
+      <c r="E304">
+        <v>37.299999999999997</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5">
+      <c r="A305" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B305" t="s">
+        <v>7</v>
+      </c>
+      <c r="C305">
+        <f t="shared" si="2"/>
+        <v>-17.008797653958947</v>
+      </c>
+      <c r="D305">
+        <v>28.3</v>
+      </c>
+      <c r="E305">
+        <v>34.1</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5">
+      <c r="A306" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B306" t="s">
+        <v>8</v>
+      </c>
+      <c r="C306">
+        <f t="shared" si="2"/>
+        <v>-18.708827404479578</v>
+      </c>
+      <c r="D306">
+        <v>185.1</v>
+      </c>
+      <c r="E306">
+        <v>227.7</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5">
+      <c r="A307" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B307" t="s">
+        <v>9</v>
+      </c>
+      <c r="C307">
+        <f t="shared" si="2"/>
+        <v>-4.9855330514133174</v>
+      </c>
+      <c r="D307">
+        <v>426.9</v>
+      </c>
+      <c r="E307">
+        <v>449.3</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5">
+      <c r="A308" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B308" t="s">
+        <v>10</v>
+      </c>
+      <c r="C308">
+        <f t="shared" si="2"/>
+        <v>-38.847117794486216</v>
+      </c>
+      <c r="D308">
+        <v>24.4</v>
+      </c>
+      <c r="E308">
+        <v>39.9</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5">
+      <c r="A309" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B309" t="s">
+        <v>11</v>
+      </c>
+      <c r="C309">
+        <f t="shared" si="2"/>
+        <v>-29.203539823008846</v>
+      </c>
+      <c r="D309">
+        <v>24</v>
+      </c>
+      <c r="E309">
+        <v>33.9</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5">
+      <c r="A310" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B310" t="s">
+        <v>12</v>
+      </c>
+      <c r="C310">
+        <f t="shared" si="2"/>
+        <v>-32.323232323232318</v>
+      </c>
+      <c r="D310">
+        <v>120.6</v>
+      </c>
+      <c r="E310">
+        <v>178.2</v>
+      </c>
+    </row>
+    <row r="311" spans="1:5">
+      <c r="A311" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B311" t="s">
+        <v>13</v>
+      </c>
+      <c r="C311">
+        <f t="shared" si="2"/>
+        <v>9.1779728651237154</v>
+      </c>
+      <c r="D311">
+        <v>136.80000000000001</v>
+      </c>
+      <c r="E311">
+        <v>125.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>